<commit_message>
long profile tprobe plots
Plots of longitudinal topography for each temperature probe
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
+++ b/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD1D74B-BF3C-4EB1-938C-347B97608B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88FFCF3-0FB3-4EA7-9943-8CF2D2295C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" firstSheet="12" activeTab="23" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" firstSheet="7" activeTab="24" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
   </bookViews>
   <sheets>
     <sheet name="Piezo 1" sheetId="1" r:id="rId1"/>
@@ -605,7 +605,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -725,11 +725,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -795,6 +808,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2208,7 +2224,7 @@
                   <c:v>2734.1680000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2734.1869999999999</c:v>
+                  <c:v>2734.1570000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>2734.114</c:v>
@@ -7924,13 +7940,13 @@
                   <c:v>2723.7240000000002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2723.7810000000004</c:v>
+                  <c:v>2723.7510000000002</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>2723.7290000000003</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2723.7750000000001</c:v>
+                  <c:v>2723.7650000000003</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>2723.7700000000004</c:v>
@@ -17181,7 +17197,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17799,7 +17815,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18485,14 +18501,14 @@
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2">
-        <v>2.0529999999999999</v>
+        <v>2.0830000000000002</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="6">
-        <f t="shared" si="0"/>
-        <v>2723.7810000000004</v>
+        <f>$F$2-C38</f>
+        <v>2723.7510000000002</v>
       </c>
       <c r="H38">
         <v>2723.7809999999999</v>
@@ -18525,14 +18541,14 @@
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2">
-        <v>2.0590000000000002</v>
+        <v>2.069</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="6">
         <f>$F$2-C40</f>
-        <v>2723.7750000000001</v>
+        <v>2723.7650000000003</v>
       </c>
       <c r="H40">
         <v>2723.7809999999999</v>
@@ -18827,7 +18843,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18874,11 +18890,11 @@
         <v>14</v>
       </c>
       <c r="F2" s="2">
-        <v>2725.8340000000003</v>
+        <v>2725.8339999999998</v>
       </c>
       <c r="G2" s="6">
         <f>$F$2-C2</f>
-        <v>2724.2590000000005</v>
+        <v>2724.259</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -18895,7 +18911,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="6">
         <f t="shared" ref="G3:G35" si="0">$F$2-C3</f>
-        <v>2724.2190000000005</v>
+        <v>2724.2190000000001</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -18914,7 +18930,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1490000000003</v>
+        <v>2724.1489999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -18931,7 +18947,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="6">
         <f t="shared" si="0"/>
-        <v>2724.0990000000002</v>
+        <v>2724.0989999999997</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -18948,7 +18964,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="6">
         <f t="shared" si="0"/>
-        <v>2724.09</v>
+        <v>2724.0899999999997</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -18965,7 +18981,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>2724.0880000000002</v>
+        <v>2724.0879999999997</v>
       </c>
       <c r="I7" t="s">
         <v>143</v>
@@ -18987,14 +19003,14 @@
       <c r="F8" s="2"/>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
-        <v>2724.0150000000003</v>
+        <v>2724.0149999999999</v>
       </c>
       <c r="H8" s="16">
         <v>2724.2139999999995</v>
       </c>
       <c r="I8" s="5">
         <f>H8-G8</f>
-        <v>0.19899999999915963</v>
+        <v>0.19899999999961437</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -19012,7 +19028,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="6">
         <f t="shared" si="0"/>
-        <v>2724.4880000000003</v>
+        <v>2724.4879999999998</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -19029,7 +19045,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>2724.0240000000003</v>
+        <v>2724.0239999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -19046,7 +19062,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>2724.0580000000004</v>
+        <v>2724.058</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -19063,7 +19079,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>2724.0970000000002</v>
+        <v>2724.0969999999998</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -19080,7 +19096,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1290000000004</v>
+        <v>2724.1289999999999</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -19097,7 +19113,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1550000000002</v>
+        <v>2724.1549999999997</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -19114,7 +19130,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1690000000003</v>
+        <v>2724.1689999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -19131,7 +19147,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1790000000001</v>
+        <v>2724.1789999999996</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -19148,7 +19164,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1790000000001</v>
+        <v>2724.1789999999996</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -19165,7 +19181,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1900000000005</v>
+        <v>2724.19</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -19182,7 +19198,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2060000000001</v>
+        <v>2724.2059999999997</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -19199,7 +19215,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1520000000005</v>
+        <v>2724.152</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -19216,7 +19232,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
-        <v>2724.1920000000005</v>
+        <v>2724.192</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -19233,7 +19249,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2180000000003</v>
+        <v>2724.2179999999998</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -19250,7 +19266,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2030000000004</v>
+        <v>2724.203</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -19267,7 +19283,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2220000000002</v>
+        <v>2724.2219999999998</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -19286,7 +19302,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2270000000003</v>
+        <v>2724.2269999999999</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -19303,7 +19319,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2580000000003</v>
+        <v>2724.2579999999998</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -19320,7 +19336,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2670000000003</v>
+        <v>2724.2669999999998</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -19337,7 +19353,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="6">
         <f t="shared" si="0"/>
-        <v>2724.2690000000002</v>
+        <v>2724.2689999999998</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -19354,7 +19370,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="6">
         <f t="shared" si="0"/>
-        <v>2724.3250000000003</v>
+        <v>2724.3249999999998</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -19371,7 +19387,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="6">
         <f t="shared" si="0"/>
-        <v>2724.3830000000003</v>
+        <v>2724.3829999999998</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -19388,7 +19404,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="6">
         <f t="shared" si="0"/>
-        <v>2724.5440000000003</v>
+        <v>2724.5439999999999</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -19405,7 +19421,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="6">
         <f t="shared" si="0"/>
-        <v>2724.59</v>
+        <v>2724.5899999999997</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -19422,7 +19438,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="6">
         <f t="shared" si="0"/>
-        <v>2724.6360000000004</v>
+        <v>2724.636</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -19439,7 +19455,7 @@
       <c r="F34" s="2"/>
       <c r="G34" s="6">
         <f t="shared" si="0"/>
-        <v>2724.8690000000001</v>
+        <v>2724.8689999999997</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -19458,7 +19474,7 @@
       <c r="F35" s="2"/>
       <c r="G35" s="6">
         <f t="shared" si="0"/>
-        <v>2724.9440000000004</v>
+        <v>2724.944</v>
       </c>
     </row>
   </sheetData>
@@ -19471,7 +19487,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20023,7 +20039,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20489,8 +20505,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9972100E-561A-4BD4-9E56-90A76ED10464}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20768,7 +20784,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f>$F$5-C13</f>
         <v>2732.8950000000004</v>
       </c>
       <c r="H13">
@@ -21236,7 +21252,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21353,7 +21369,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f>$F$2-C6</f>
         <v>2733.83</v>
       </c>
     </row>
@@ -21837,7 +21853,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21876,18 +21892,16 @@
         <v>145</v>
       </c>
       <c r="B2" s="6">
-        <v>1.9950000000000001</v>
+        <v>2.4449999999999998</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="6">
-        <v>1.5580000000000001</v>
-      </c>
+      <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
         <v>77</v>
       </c>
       <c r="F2" s="19">
         <f>$G$2+B2</f>
-        <v>2735.5099999999998</v>
+        <v>2735.96</v>
       </c>
       <c r="G2" s="6">
         <v>2733.5149999999999</v>
@@ -21908,7 +21922,11 @@
       <c r="F3" s="2"/>
       <c r="G3" s="2">
         <f>$F$2-C3</f>
-        <v>2733.2649999999999</v>
+        <v>2733.7150000000001</v>
+      </c>
+      <c r="H3">
+        <f>C3-0.5</f>
+        <v>1.7450000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -21926,8 +21944,12 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G22" si="0">$F$2-C4</f>
-        <v>2733.27</v>
+        <f>$F$2-C4</f>
+        <v>2733.7200000000003</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H22" si="0">C4-0.5</f>
+        <v>1.7400000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -21959,8 +21981,12 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.0559999999996</v>
+        <f t="shared" ref="G4:G22" si="2">$F$2-C6</f>
+        <v>2733.5059999999999</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.9540000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -21976,8 +22002,12 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.087</v>
+        <f t="shared" si="2"/>
+        <v>2733.5370000000003</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.923</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -21993,8 +22023,12 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.0629999999996</v>
+        <f t="shared" si="2"/>
+        <v>2733.5129999999999</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1.9470000000000001</v>
       </c>
       <c r="I8" s="11" t="s">
         <v>116</v>
@@ -22013,8 +22047,12 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.1389999999997</v>
+        <f t="shared" si="2"/>
+        <v>2733.5889999999999</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>1.871</v>
       </c>
       <c r="I9" s="11">
         <f>C11-C12</f>
@@ -22034,8 +22072,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.1259999999997</v>
+        <f t="shared" si="2"/>
+        <v>2733.576</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1.8839999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -22053,8 +22095,12 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.0959999999995</v>
+        <f t="shared" si="2"/>
+        <v>2733.5459999999998</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>1.9140000000000001</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -22071,8 +22117,12 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.2149999999997</v>
+        <f t="shared" si="2"/>
+        <v>2733.665</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1.7949999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -22088,13 +22138,17 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.0339999999997</v>
+        <f t="shared" si="2"/>
+        <v>2733.4839999999999</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>1.976</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" ref="A14:A22" si="2">A13+10</f>
+        <f t="shared" ref="A14:A22" si="3">A13+10</f>
         <v>100</v>
       </c>
       <c r="B14" s="2"/>
@@ -22105,13 +22159,17 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>2732.9839999999999</v>
+        <f t="shared" si="2"/>
+        <v>2733.4340000000002</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>2.0259999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
       <c r="B15" s="2"/>
@@ -22122,13 +22180,17 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>2732.991</v>
+        <f t="shared" si="2"/>
+        <v>2733.4410000000003</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>2.0190000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
       <c r="B16" s="2"/>
@@ -22141,13 +22203,17 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.1229999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2733.5729999999999</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>1.887</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
       <c r="B17" s="2"/>
@@ -22158,13 +22224,17 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.0759999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2733.5259999999998</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>1.9340000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
       <c r="B18" s="2"/>
@@ -22175,13 +22245,17 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.0849999999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2733.5349999999999</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>1.9249999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="B19" s="2"/>
@@ -22192,13 +22266,17 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.1809999999996</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2733.6309999999999</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>1.8290000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
       <c r="B20" s="2"/>
@@ -22209,13 +22287,17 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.1949999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2733.645</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1.8149999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
       <c r="B21" s="2"/>
@@ -22226,13 +22308,17 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.203</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>2733.6530000000002</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1.8069999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
       <c r="B22" s="2"/>
@@ -22245,8 +22331,12 @@
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <f t="shared" si="0"/>
-        <v>2733.2349999999997</v>
+        <f t="shared" si="2"/>
+        <v>2733.6849999999999</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>1.7749999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -22259,7 +22349,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22678,7 +22768,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23387,7 +23477,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23584,14 +23674,14 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
-        <v>1.952</v>
+        <v>1.982</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>2734.1869999999999</v>
+        <v>2734.1570000000002</v>
       </c>
       <c r="H10">
         <v>2734.2060000000001</v>
@@ -23929,7 +24019,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24245,14 +24335,14 @@
         <v>2721.768</v>
       </c>
       <c r="H17" s="17">
-        <v>2721.7619999999997</v>
+        <v>2721.7620000000002</v>
       </c>
       <c r="I17" s="17" t="s">
         <v>142</v>
       </c>
       <c r="J17">
         <f>H17-G17</f>
-        <v>-6.0000000003128662E-3</v>
+        <v>-5.9999999998581188E-3</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -24515,7 +24605,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24956,7 +25046,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25639,7 +25729,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26376,8 +26466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62944037-0C0F-454E-8D1D-821A1F229F1C}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27004,8 +27094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C12D5E-274C-49F4-AC1E-9E3A5CF8DFEE}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27528,8 +27618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15857BB-7009-42F0-BB33-F587ED47BBA2}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27595,7 +27685,7 @@
         <v>107</v>
       </c>
       <c r="B2" s="6">
-        <v>2.411</v>
+        <v>2.6909999999999998</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6">
@@ -27604,7 +27694,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6">
         <f>$G$2+B2</f>
-        <v>2739.8669999999997</v>
+        <v>2740.1469999999995</v>
       </c>
       <c r="G2" s="6">
         <f>2737.593-D2</f>
@@ -27614,14 +27704,14 @@
         <v>144</v>
       </c>
       <c r="L2" s="2">
-        <v>2.5449999999999999</v>
+        <v>3.165</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="6">
         <f>Q2+L2</f>
-        <v>2739.56</v>
+        <v>2740.18</v>
       </c>
       <c r="Q2" s="6">
         <v>2737.0149999999999</v>
@@ -27642,7 +27732,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="6">
         <f>$F$2-C3</f>
-        <v>2738.2489999999998</v>
+        <v>2738.5289999999995</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>131</v>
@@ -27658,7 +27748,7 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="2">
         <f>$P$2-M3</f>
-        <v>2738.0369999999998</v>
+        <v>2738.6569999999997</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -27675,7 +27765,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="6">
         <f t="shared" ref="G4:G26" si="0">$F$2-C4</f>
-        <v>2738.2129999999997</v>
+        <v>2738.4929999999995</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>133</v>
@@ -27689,7 +27779,7 @@
       <c r="P4" s="3"/>
       <c r="Q4" s="2">
         <f t="shared" ref="Q4:Q29" si="1">$P$2-M4</f>
-        <v>2738.0320000000002</v>
+        <v>2738.652</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -27706,7 +27796,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="6">
         <f t="shared" si="0"/>
-        <v>2738.0629999999996</v>
+        <v>2738.3429999999994</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>134</v>
@@ -27720,7 +27810,7 @@
       <c r="P5" s="3"/>
       <c r="Q5" s="2">
         <f t="shared" si="1"/>
-        <v>2738</v>
+        <v>2738.62</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -27737,7 +27827,7 @@
       <c r="F6" s="2"/>
       <c r="G6" s="6">
         <f t="shared" si="0"/>
-        <v>2738.0029999999997</v>
+        <v>2738.2829999999994</v>
       </c>
       <c r="K6" s="2">
         <v>1.2</v>
@@ -27751,7 +27841,7 @@
       <c r="P6" s="3"/>
       <c r="Q6" s="2">
         <f t="shared" si="1"/>
-        <v>2737.9639999999999</v>
+        <v>2738.5839999999998</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -27768,7 +27858,7 @@
       <c r="F7" s="2"/>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>2737.9969999999998</v>
+        <v>2738.2769999999996</v>
       </c>
       <c r="K7" s="2">
         <v>1.3</v>
@@ -27782,7 +27872,7 @@
       <c r="P7" s="3"/>
       <c r="Q7" s="2">
         <f t="shared" si="1"/>
-        <v>2737.92</v>
+        <v>2738.54</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -27801,7 +27891,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
-        <v>2737.9769999999999</v>
+        <v>2738.2569999999996</v>
       </c>
       <c r="K8" s="2">
         <v>1.4</v>
@@ -27815,7 +27905,7 @@
       <c r="P8" s="3"/>
       <c r="Q8" s="2">
         <f t="shared" si="1"/>
-        <v>2737.91</v>
+        <v>2738.5299999999997</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -27832,7 +27922,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="6">
         <f t="shared" si="0"/>
-        <v>2737.9609999999998</v>
+        <v>2738.2409999999995</v>
       </c>
       <c r="I9" s="11" t="s">
         <v>117</v>
@@ -27849,7 +27939,7 @@
       <c r="P9" s="3"/>
       <c r="Q9" s="2">
         <f t="shared" si="1"/>
-        <v>2737.8910000000001</v>
+        <v>2738.511</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -27866,7 +27956,7 @@
       <c r="F10" s="2"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>2737.9929999999999</v>
+        <v>2738.2729999999997</v>
       </c>
       <c r="I10" s="11">
         <f>C20-C21</f>
@@ -27886,7 +27976,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="2">
         <f t="shared" si="1"/>
-        <v>2737.7620000000002</v>
+        <v>2738.3820000000001</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -27903,7 +27993,7 @@
       <c r="F11" s="2"/>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>2737.9719999999998</v>
+        <v>2738.2519999999995</v>
       </c>
       <c r="K11" s="2">
         <v>1.7</v>
@@ -27917,7 +28007,7 @@
       <c r="P11" s="3"/>
       <c r="Q11" s="2">
         <f t="shared" si="1"/>
-        <v>2737.7359999999999</v>
+        <v>2738.3559999999998</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
@@ -27934,7 +28024,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>2738.0539999999996</v>
+        <v>2738.3339999999994</v>
       </c>
       <c r="I12" s="11" t="s">
         <v>130</v>
@@ -27953,7 +28043,7 @@
       <c r="P12" s="3"/>
       <c r="Q12" s="2">
         <f t="shared" si="1"/>
-        <v>2737.8249999999998</v>
+        <v>2738.4449999999997</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -27970,7 +28060,7 @@
       <c r="F13" s="2"/>
       <c r="G13" s="6">
         <f t="shared" si="0"/>
-        <v>2738.0419999999999</v>
+        <v>2738.3219999999997</v>
       </c>
       <c r="I13" s="11">
         <f>M17-M18</f>
@@ -27988,7 +28078,7 @@
       <c r="P13" s="3"/>
       <c r="Q13" s="2">
         <f t="shared" si="1"/>
-        <v>2737.806</v>
+        <v>2738.4259999999999</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -28007,7 +28097,7 @@
       <c r="F14" s="2"/>
       <c r="G14" s="6">
         <f t="shared" si="0"/>
-        <v>2738.1649999999995</v>
+        <v>2738.4449999999993</v>
       </c>
       <c r="K14" s="2">
         <v>2</v>
@@ -28021,7 +28111,7 @@
       <c r="P14" s="3"/>
       <c r="Q14" s="2">
         <f t="shared" si="1"/>
-        <v>2737.7150000000001</v>
+        <v>2738.335</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -28038,7 +28128,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="6">
         <f t="shared" si="0"/>
-        <v>2738.1319999999996</v>
+        <v>2738.4119999999994</v>
       </c>
       <c r="K15" s="2">
         <v>2.1</v>
@@ -28052,7 +28142,7 @@
       <c r="P15" s="3"/>
       <c r="Q15" s="2">
         <f t="shared" si="1"/>
-        <v>2737.7359999999999</v>
+        <v>2738.3559999999998</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
@@ -28069,7 +28159,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="6">
         <f t="shared" si="0"/>
-        <v>2738.1189999999997</v>
+        <v>2738.3989999999994</v>
       </c>
       <c r="K16" s="2">
         <v>2.2000000000000002</v>
@@ -28083,7 +28173,7 @@
       <c r="P16" s="3"/>
       <c r="Q16" s="2">
         <f t="shared" si="1"/>
-        <v>2737.6979999999999</v>
+        <v>2738.3179999999998</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -28100,7 +28190,7 @@
       <c r="F17" s="2"/>
       <c r="G17" s="6">
         <f t="shared" si="0"/>
-        <v>2738.0509999999999</v>
+        <v>2738.3309999999997</v>
       </c>
       <c r="K17" s="2">
         <v>2.25</v>
@@ -28116,7 +28206,7 @@
       <c r="P17" s="3"/>
       <c r="Q17" s="2">
         <f t="shared" si="1"/>
-        <v>2737.6950000000002</v>
+        <v>2738.3150000000001</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -28133,7 +28223,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="6">
         <f t="shared" si="0"/>
-        <v>2738.0319999999997</v>
+        <v>2738.3119999999994</v>
       </c>
       <c r="K18" s="2">
         <v>2.25</v>
@@ -28149,7 +28239,7 @@
       <c r="P18" s="3"/>
       <c r="Q18" s="2">
         <f t="shared" si="1"/>
-        <v>2737.8879999999999</v>
+        <v>2738.5079999999998</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -28166,7 +28256,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="6">
         <f t="shared" si="0"/>
-        <v>2737.9549999999999</v>
+        <v>2738.2349999999997</v>
       </c>
       <c r="K19" s="2">
         <v>2.2999999999999998</v>
@@ -28180,7 +28270,7 @@
       <c r="P19" s="3"/>
       <c r="Q19" s="2">
         <f t="shared" si="1"/>
-        <v>2737.7</v>
+        <v>2738.3199999999997</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
@@ -28199,7 +28289,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="6">
         <f t="shared" si="0"/>
-        <v>2737.9459999999999</v>
+        <v>2738.2259999999997</v>
       </c>
       <c r="K20" s="2">
         <v>2.4</v>
@@ -28215,7 +28305,7 @@
       <c r="P20" s="3"/>
       <c r="Q20" s="2">
         <f t="shared" si="1"/>
-        <v>2737.8150000000001</v>
+        <v>2738.4349999999999</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
@@ -28233,7 +28323,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="6">
         <f t="shared" si="0"/>
-        <v>2738.194</v>
+        <v>2738.4739999999997</v>
       </c>
       <c r="K21" s="2">
         <v>2.5</v>
@@ -28247,7 +28337,7 @@
       <c r="P21" s="3"/>
       <c r="Q21" s="2">
         <f t="shared" si="1"/>
-        <v>2737.72</v>
+        <v>2738.3399999999997</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
@@ -28266,7 +28356,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="6">
         <f t="shared" si="0"/>
-        <v>2738.0119999999997</v>
+        <v>2738.2919999999995</v>
       </c>
       <c r="K22" s="2">
         <v>2.6</v>
@@ -28280,7 +28370,7 @@
       <c r="P22" s="3"/>
       <c r="Q22" s="2">
         <f t="shared" si="1"/>
-        <v>2737.8049999999998</v>
+        <v>2738.4249999999997</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
@@ -28297,7 +28387,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="6">
         <f t="shared" si="0"/>
-        <v>2738.1359999999995</v>
+        <v>2738.4159999999993</v>
       </c>
       <c r="K23" s="2">
         <v>2.7</v>
@@ -28311,7 +28401,7 @@
       <c r="P23" s="3"/>
       <c r="Q23" s="2">
         <f t="shared" si="1"/>
-        <v>2737.79</v>
+        <v>2738.41</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
@@ -28328,7 +28418,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="6">
         <f t="shared" si="0"/>
-        <v>2738.1879999999996</v>
+        <v>2738.4679999999994</v>
       </c>
       <c r="K24" s="2">
         <v>2.8</v>
@@ -28342,7 +28432,7 @@
       <c r="P24" s="3"/>
       <c r="Q24" s="2">
         <f t="shared" si="1"/>
-        <v>2737.8049999999998</v>
+        <v>2738.4249999999997</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
@@ -28359,7 +28449,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="6">
         <f t="shared" si="0"/>
-        <v>2738.1829999999995</v>
+        <v>2738.4629999999993</v>
       </c>
       <c r="K25" s="2">
         <v>2.9</v>
@@ -28375,7 +28465,7 @@
       <c r="P25" s="3"/>
       <c r="Q25" s="2">
         <f t="shared" si="1"/>
-        <v>2737.817</v>
+        <v>2738.4369999999999</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
@@ -28394,7 +28484,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="6">
         <f t="shared" si="0"/>
-        <v>2738.1769999999997</v>
+        <v>2738.4569999999994</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>137</v>
@@ -28408,7 +28498,7 @@
       <c r="P26" s="3"/>
       <c r="Q26" s="2">
         <f t="shared" si="1"/>
-        <v>2737.84</v>
+        <v>2738.46</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -28431,7 +28521,7 @@
       <c r="P27" s="3"/>
       <c r="Q27" s="2">
         <f t="shared" si="1"/>
-        <v>2737.915</v>
+        <v>2738.5349999999999</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -28449,7 +28539,7 @@
       <c r="P28" s="3"/>
       <c r="Q28" s="2">
         <f t="shared" si="1"/>
-        <v>2737.9349999999999</v>
+        <v>2738.5549999999998</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -28467,7 +28557,7 @@
       <c r="P29" s="3"/>
       <c r="Q29" s="2">
         <f t="shared" si="1"/>
-        <v>2737.9749999999999</v>
+        <v>2738.5949999999998</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -28491,8 +28581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278C6A75-EB2C-4F06-8258-6CEC79F84880}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29313,8 +29403,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF970D2A-25F7-43D8-9437-28DE93019D3F}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30309,7 +30399,7 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30334,7 +30424,7 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
@@ -30376,19 +30466,19 @@
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="6">
-        <v>3.226</v>
+      <c r="C2" s="2">
+        <v>3.3260000000000001</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="F2" s="6">
-        <v>2725.9459999999995</v>
+        <v>2725.9459999999999</v>
       </c>
       <c r="G2" s="6">
         <f>$F$2-C2</f>
-        <v>2722.7199999999993</v>
+        <v>2722.62</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>121</v>
@@ -30416,14 +30506,14 @@
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2">
-        <v>3.2480000000000002</v>
+        <v>3.3480000000000003</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1"/>
       <c r="F3" s="2"/>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G31" si="0">$F$2-C3</f>
-        <v>2722.6979999999994</v>
+        <f t="shared" ref="G3:G12" si="0">$F$2-C3</f>
+        <v>2722.598</v>
       </c>
       <c r="K3" s="2">
         <v>0</v>
@@ -30449,14 +30539,14 @@
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2">
-        <v>3.2469999999999999</v>
+        <v>3.347</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="6">
         <f t="shared" si="0"/>
-        <v>2722.6989999999996</v>
+        <v>2722.5989999999997</v>
       </c>
       <c r="K4" s="2">
         <v>10</v>
@@ -30480,7 +30570,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2">
-        <v>3.3149999999999999</v>
+        <v>3.415</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
@@ -30489,7 +30579,7 @@
       <c r="F5" s="2"/>
       <c r="G5" s="6">
         <f t="shared" si="0"/>
-        <v>2722.6309999999994</v>
+        <v>2722.5309999999999</v>
       </c>
       <c r="K5" s="2">
         <v>20</v>
@@ -30513,14 +30603,14 @@
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2">
-        <v>3.3159999999999998</v>
+        <v>3.4159999999999999</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="6">
         <f t="shared" si="0"/>
-        <v>2722.6299999999997</v>
+        <v>2722.5299999999997</v>
       </c>
       <c r="K6" s="2">
         <v>30</v>
@@ -30544,14 +30634,14 @@
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2">
-        <v>3.331</v>
+        <v>3.431</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="6">
         <f t="shared" si="0"/>
-        <v>2722.6149999999993</v>
+        <v>2722.5149999999999</v>
       </c>
       <c r="K7" s="2">
         <v>40</v>
@@ -30575,14 +30665,14 @@
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2">
-        <v>3.3620000000000001</v>
+        <v>3.4620000000000002</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="6">
         <f t="shared" si="0"/>
-        <v>2722.5839999999994</v>
+        <v>2722.4839999999999</v>
       </c>
       <c r="K8" s="2">
         <v>50</v>
@@ -30606,14 +30696,14 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2">
-        <v>3.3319999999999999</v>
+        <v>3.4319999999999999</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="6">
         <f t="shared" si="0"/>
-        <v>2722.6139999999996</v>
+        <v>2722.5140000000001</v>
       </c>
       <c r="K9" s="2">
         <v>60</v>
@@ -30643,14 +30733,14 @@
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2">
-        <v>3.3370000000000002</v>
+        <v>3.4370000000000003</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="6">
         <f t="shared" si="0"/>
-        <v>2722.6089999999995</v>
+        <v>2722.509</v>
       </c>
       <c r="K10" s="2">
         <v>70</v>
@@ -30683,14 +30773,14 @@
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2">
-        <v>3.3450000000000002</v>
+        <v>3.4450000000000003</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="6">
         <f t="shared" si="0"/>
-        <v>2722.6009999999997</v>
+        <v>2722.5009999999997</v>
       </c>
       <c r="K11" s="2">
         <v>70</v>
@@ -30716,14 +30806,14 @@
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2">
-        <v>3.76</v>
+        <v>3.86</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="6">
         <f t="shared" si="0"/>
-        <v>2722.1859999999992</v>
+        <v>2722.0859999999998</v>
       </c>
       <c r="K12" s="2">
         <v>80</v>
@@ -30778,7 +30868,7 @@
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2">
-        <v>3.3330000000000002</v>
+        <v>3.4330000000000003</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
@@ -30786,12 +30876,12 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6129999999994</v>
+        <f>$F$2-C14</f>
+        <v>2722.5129999999999</v>
       </c>
       <c r="I14" s="11">
-        <f>C14-C15</f>
-        <v>0.13900000000000023</v>
+        <f>G15-G14</f>
+        <v>0.13900000000012369</v>
       </c>
       <c r="K14" s="2">
         <v>100</v>
@@ -30814,7 +30904,7 @@
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2">
-        <v>3.194</v>
+        <v>3.294</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
@@ -30822,8 +30912,8 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.7519999999995</v>
+        <f t="shared" ref="G15:G31" si="3">$F$2-C15</f>
+        <v>2722.652</v>
       </c>
       <c r="K15" s="2">
         <v>110</v>
@@ -30847,14 +30937,14 @@
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2">
-        <v>3.3559999999999999</v>
+        <v>3.456</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.5899999999992</v>
+        <f t="shared" si="3"/>
+        <v>2722.49</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>130</v>
@@ -30876,19 +30966,19 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" ref="A17:A31" si="3">A16+10</f>
+        <f t="shared" ref="A17:A31" si="4">A16+10</f>
         <v>140</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2">
-        <v>3.355</v>
+        <v>3.4550000000000001</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.5909999999994</v>
+        <f t="shared" si="3"/>
+        <v>2722.491</v>
       </c>
       <c r="I17" s="11">
         <f>M10-M11</f>
@@ -30913,19 +31003,19 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2">
-        <v>3.3439999999999999</v>
+        <v>3.444</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6019999999994</v>
+        <f t="shared" si="3"/>
+        <v>2722.502</v>
       </c>
       <c r="K18" s="2">
         <v>140</v>
@@ -30944,19 +31034,19 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2">
-        <v>3.3159999999999998</v>
+        <v>3.4159999999999999</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6299999999997</v>
+        <f t="shared" si="3"/>
+        <v>2722.5299999999997</v>
       </c>
       <c r="K19" s="2">
         <v>150</v>
@@ -30975,12 +31065,12 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>170</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2">
-        <v>3.3140000000000001</v>
+        <v>3.4140000000000001</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
@@ -30988,8 +31078,8 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6319999999996</v>
+        <f t="shared" si="3"/>
+        <v>2722.5319999999997</v>
       </c>
       <c r="K20" s="2">
         <v>160</v>
@@ -31008,19 +31098,19 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2">
-        <v>3.2879999999999998</v>
+        <v>3.3879999999999999</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6579999999994</v>
+        <f t="shared" si="3"/>
+        <v>2722.558</v>
       </c>
       <c r="K21" s="2">
         <v>170</v>
@@ -31039,19 +31129,19 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>190</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2">
-        <v>3.2890000000000001</v>
+        <v>3.3890000000000002</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6569999999992</v>
+        <f t="shared" si="3"/>
+        <v>2722.5569999999998</v>
       </c>
       <c r="K22" s="2">
         <v>180</v>
@@ -31070,19 +31160,19 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>200</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2">
-        <v>3.2549999999999999</v>
+        <v>3.355</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6909999999993</v>
+        <f t="shared" si="3"/>
+        <v>2722.5909999999999</v>
       </c>
       <c r="K23" s="2">
         <v>190</v>
@@ -31101,19 +31191,19 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>210</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2">
-        <v>3.274</v>
+        <v>3.3740000000000001</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6719999999996</v>
+        <f t="shared" si="3"/>
+        <v>2722.5720000000001</v>
       </c>
       <c r="K24" s="2">
         <v>200</v>
@@ -31132,36 +31222,36 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>220</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2">
-        <v>3.2679999999999998</v>
+        <v>3.3679999999999999</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6779999999994</v>
+        <f t="shared" si="3"/>
+        <v>2722.578</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>230</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2">
-        <v>3.2509999999999999</v>
+        <v>3.351</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.6949999999993</v>
+        <f t="shared" si="3"/>
+        <v>2722.5949999999998</v>
       </c>
       <c r="K26" s="24" t="s">
         <v>129</v>
@@ -31175,30 +31265,30 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2">
-        <v>3.2410000000000001</v>
+        <v>3.3410000000000002</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.7049999999995</v>
+        <f t="shared" si="3"/>
+        <v>2722.605</v>
       </c>
       <c r="O27" s="23"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2">
-        <v>3.0190000000000001</v>
+        <v>3.1190000000000002</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
@@ -31206,55 +31296,55 @@
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.9269999999997</v>
+        <f t="shared" si="3"/>
+        <v>2722.8269999999998</v>
       </c>
       <c r="O28" s="23"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>260</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2">
-        <v>3.0139999999999998</v>
+        <v>3.1139999999999999</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.9319999999993</v>
+        <f t="shared" si="3"/>
+        <v>2722.8319999999999</v>
       </c>
       <c r="O29" s="23"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>270</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2">
-        <v>2.9790000000000001</v>
+        <v>3.0790000000000002</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="6">
-        <f t="shared" si="0"/>
-        <v>2722.9669999999996</v>
+        <f t="shared" si="3"/>
+        <v>2722.8669999999997</v>
       </c>
       <c r="O30" s="23"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>280</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2">
-        <v>2.9319999999999999</v>
+        <v>3.032</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
@@ -31262,8 +31352,8 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="6">
-        <f t="shared" si="0"/>
-        <v>2723.0139999999997</v>
+        <f t="shared" si="3"/>
+        <v>2722.9139999999998</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
@@ -31288,7 +31378,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31918,7 +32008,7 @@
   <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32512,7 +32602,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33321,7 +33411,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
re-did barometric compensation for the piezometers
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
+++ b/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88FFCF3-0FB3-4EA7-9943-8CF2D2295C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DD2D8C-F492-4CF4-BC23-E43D9896A63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" firstSheet="7" activeTab="24" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="804" firstSheet="7" activeTab="23" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
   </bookViews>
   <sheets>
     <sheet name="Piezo 1" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
     <t>bottom piezo 6</t>
   </si>
   <si>
-    <t>top piezo 6</t>
+    <t>top piezo 6 c</t>
   </si>
 </sst>
 </file>
@@ -742,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -801,16 +801,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -900,7 +897,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1290,7 +1287,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1680724640"/>
@@ -1352,7 +1349,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1680722144"/>
@@ -1400,7 +1397,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1932,7 +1929,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1568800591"/>
@@ -1994,7 +1991,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015223983"/>
@@ -2042,7 +2039,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2505,7 +2502,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="583681535"/>
@@ -2567,7 +2564,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811039471"/>
@@ -2615,7 +2612,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3171,7 +3168,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1701696767"/>
@@ -3233,7 +3230,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1869339711"/>
@@ -3281,7 +3278,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3828,7 +3825,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584295391"/>
@@ -3890,7 +3887,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1869286815"/>
@@ -3938,7 +3935,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3989,7 +3986,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4292,7 +4289,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1753949856"/>
@@ -4354,7 +4351,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1753949024"/>
@@ -4402,7 +4399,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5018,7 +5015,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2043194127"/>
@@ -5080,7 +5077,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015234655"/>
@@ -5128,7 +5125,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5777,7 +5774,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1810760255"/>
@@ -5839,7 +5836,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811056175"/>
@@ -5887,7 +5884,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6418,7 +6415,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1993662911"/>
@@ -6480,7 +6477,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811060815"/>
@@ -6528,7 +6525,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6903,7 +6900,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1273530959"/>
@@ -6966,7 +6963,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1273528463"/>
@@ -7014,7 +7011,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7065,7 +7062,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7483,7 +7480,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1946070992"/>
@@ -7545,7 +7542,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1645237152"/>
@@ -7593,7 +7590,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8251,7 +8248,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1988108927"/>
@@ -8313,7 +8310,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811050607"/>
@@ -8361,7 +8358,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8872,7 +8869,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2008535167"/>
@@ -8934,7 +8931,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811067311"/>
@@ -8982,7 +8979,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -21252,7 +21249,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21981,7 +21978,7 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" ref="G4:G22" si="2">$F$2-C6</f>
+        <f t="shared" ref="G6:G22" si="2">$F$2-C6</f>
         <v>2733.5059999999999</v>
       </c>
       <c r="H6">
@@ -26466,8 +26463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62944037-0C0F-454E-8D1D-821A1F229F1C}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27054,11 +27051,11 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="22">
+      <c r="A35" s="2">
         <v>410</v>
       </c>
       <c r="B35" s="3"/>
-      <c r="C35" s="22">
+      <c r="C35" s="2">
         <v>2.4750000000000001</v>
       </c>
       <c r="D35" s="3"/>
@@ -27070,11 +27067,11 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="22">
+      <c r="A36" s="2">
         <v>430</v>
       </c>
       <c r="B36" s="3"/>
-      <c r="C36" s="22">
+      <c r="C36" s="2">
         <v>2.2749999999999999</v>
       </c>
       <c r="D36" s="3"/>
@@ -27094,8 +27091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C12D5E-274C-49F4-AC1E-9E3A5CF8DFEE}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27618,7 +27615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15857BB-7009-42F0-BB33-F587ED47BBA2}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -30424,7 +30421,7 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="22" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">

</xml_diff>

<commit_message>
calculated bed perimeters for baskets
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
+++ b/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DD2D8C-F492-4CF4-BC23-E43D9896A63B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3082D-E847-4C25-AD8B-4B69B0E1B242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="804" firstSheet="7" activeTab="23" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
+    <workbookView xWindow="-24135" yWindow="315" windowWidth="22260" windowHeight="14940" tabRatio="804" firstSheet="12" activeTab="24" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
   </bookViews>
   <sheets>
     <sheet name="Piezo 1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="165">
   <si>
     <t>Distance</t>
   </si>
@@ -471,9 +471,6 @@
     <t>Top of  rock</t>
   </si>
   <si>
-    <t>3m</t>
-  </si>
-  <si>
     <t>Vegetation</t>
   </si>
   <si>
@@ -605,7 +602,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -725,19 +722,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -801,7 +785,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -897,7 +881,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1287,7 +1271,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1680724640"/>
@@ -1349,7 +1333,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1680722144"/>
@@ -1397,7 +1381,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1929,7 +1913,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1568800591"/>
@@ -1991,7 +1975,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015223983"/>
@@ -2039,7 +2023,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2502,7 +2486,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="583681535"/>
@@ -2564,7 +2548,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811039471"/>
@@ -2612,7 +2596,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3168,7 +3152,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1701696767"/>
@@ -3230,7 +3214,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1869339711"/>
@@ -3278,7 +3262,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3825,7 +3809,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584295391"/>
@@ -3887,7 +3871,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1869286815"/>
@@ -3935,7 +3919,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3986,7 +3970,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4289,7 +4273,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1753949856"/>
@@ -4351,7 +4335,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1753949024"/>
@@ -4399,7 +4383,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5015,7 +4999,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2043194127"/>
@@ -5077,7 +5061,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015234655"/>
@@ -5125,7 +5109,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5774,7 +5758,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1810760255"/>
@@ -5836,7 +5820,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811056175"/>
@@ -5884,7 +5868,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6415,7 +6399,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1993662911"/>
@@ -6477,7 +6461,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811060815"/>
@@ -6525,7 +6509,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6900,7 +6884,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1273530959"/>
@@ -6963,7 +6947,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1273528463"/>
@@ -7011,7 +6995,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7062,7 +7046,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-AR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7480,7 +7464,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1946070992"/>
@@ -7542,7 +7526,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1645237152"/>
@@ -7590,7 +7574,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8248,7 +8232,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1988108927"/>
@@ -8310,7 +8294,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811050607"/>
@@ -8358,7 +8342,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8869,7 +8853,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2008535167"/>
@@ -8931,7 +8915,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-AR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811067311"/>
@@ -8979,7 +8963,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="es-AR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -18981,7 +18965,7 @@
         <v>2724.0879999999997</v>
       </c>
       <c r="I7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -19484,7 +19468,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19566,7 +19550,10 @@
         <f>A3+10</f>
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <f>A4/100</f>
+        <v>0.1</v>
+      </c>
       <c r="C4" s="2">
         <v>2.1850000000000001</v>
       </c>
@@ -19583,7 +19570,10 @@
         <f t="shared" ref="A5:A18" si="1">A4+10</f>
         <v>20</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <f t="shared" ref="B5:B29" si="2">A5/100</f>
+        <v>0.2</v>
+      </c>
       <c r="C5" s="2">
         <v>2.25</v>
       </c>
@@ -19600,7 +19590,10 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
       <c r="C6" s="2">
         <v>2.238</v>
       </c>
@@ -19617,7 +19610,10 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
       <c r="C7" s="2">
         <v>2.2360000000000002</v>
       </c>
@@ -19634,7 +19630,10 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
       <c r="C8" s="2">
         <v>2.327</v>
       </c>
@@ -19653,7 +19652,10 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
       <c r="C9" s="2">
         <v>2.3849999999999998</v>
       </c>
@@ -19670,7 +19672,10 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
       <c r="C10" s="2">
         <v>2.3679999999999999</v>
       </c>
@@ -19687,7 +19692,10 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
       <c r="C11" s="2">
         <v>2.34</v>
       </c>
@@ -19707,7 +19715,10 @@
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
       <c r="C12" s="2">
         <v>2.3660000000000001</v>
       </c>
@@ -19728,7 +19739,10 @@
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="C13" s="2">
         <v>2.3860000000000001</v>
       </c>
@@ -19745,7 +19759,10 @@
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C14" s="2">
         <v>2.4049999999999998</v>
       </c>
@@ -19762,7 +19779,10 @@
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
       <c r="C15" s="2">
         <v>2.4249999999999998</v>
       </c>
@@ -19779,7 +19799,10 @@
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3</v>
+      </c>
       <c r="C16" s="2">
         <v>2.4159999999999999</v>
       </c>
@@ -19796,7 +19819,10 @@
         <f t="shared" si="1"/>
         <v>140</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
       <c r="C17" s="2">
         <v>2.4209999999999998</v>
       </c>
@@ -19813,7 +19839,10 @@
         <f t="shared" si="1"/>
         <v>150</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
       <c r="C18" s="2">
         <v>2.4590000000000001</v>
       </c>
@@ -19831,7 +19860,10 @@
       <c r="A19" s="2">
         <v>150</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
       <c r="C19" s="2">
         <v>2.234</v>
       </c>
@@ -19857,7 +19889,10 @@
         <f>A18+10</f>
         <v>160</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
       <c r="C20" s="2">
         <v>2.3679999999999999</v>
       </c>
@@ -19873,10 +19908,13 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" ref="A21:A26" si="2">A20+10</f>
+        <f t="shared" ref="A21:A26" si="3">A20+10</f>
         <v>170</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7</v>
+      </c>
       <c r="C21" s="2">
         <v>2.2250000000000001</v>
       </c>
@@ -19890,10 +19928,13 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="B22" s="2">
         <f t="shared" si="2"/>
-        <v>180</v>
-      </c>
-      <c r="B22" s="2"/>
+        <v>1.8</v>
+      </c>
       <c r="C22" s="2">
         <v>2.2240000000000002</v>
       </c>
@@ -19907,10 +19948,13 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
+        <f t="shared" si="3"/>
+        <v>190</v>
+      </c>
+      <c r="B23" s="2">
         <f t="shared" si="2"/>
-        <v>190</v>
-      </c>
-      <c r="B23" s="2"/>
+        <v>1.9</v>
+      </c>
       <c r="C23" s="2">
         <v>2.0070000000000001</v>
       </c>
@@ -19924,10 +19968,13 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
+        <f t="shared" si="3"/>
+        <v>200</v>
+      </c>
+      <c r="B24" s="2">
         <f t="shared" si="2"/>
-        <v>200</v>
-      </c>
-      <c r="B24" s="2"/>
+        <v>2</v>
+      </c>
       <c r="C24" s="2">
         <v>2.105</v>
       </c>
@@ -19941,10 +19988,13 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
+        <f t="shared" si="3"/>
+        <v>210</v>
+      </c>
+      <c r="B25" s="2">
         <f t="shared" si="2"/>
-        <v>210</v>
-      </c>
-      <c r="B25" s="2"/>
+        <v>2.1</v>
+      </c>
       <c r="C25" s="2">
         <v>2.1110000000000002</v>
       </c>
@@ -19958,10 +20008,13 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
+        <f t="shared" si="3"/>
+        <v>220</v>
+      </c>
+      <c r="B26" s="2">
         <f t="shared" si="2"/>
-        <v>220</v>
-      </c>
-      <c r="B26" s="2"/>
+        <v>2.2000000000000002</v>
+      </c>
       <c r="C26" s="2">
         <v>2.0059999999999998</v>
       </c>
@@ -19975,10 +20028,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" ref="A27:A29" si="3">A26+10</f>
+        <f t="shared" ref="A27:A29" si="4">A26+10</f>
         <v>230</v>
       </c>
-      <c r="B27" s="2"/>
+      <c r="B27" s="2">
+        <f t="shared" si="2"/>
+        <v>2.2999999999999998</v>
+      </c>
       <c r="C27" s="2">
         <v>1.968</v>
       </c>
@@ -19992,10 +20048,13 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
-      <c r="B28" s="2"/>
+      <c r="B28" s="2">
+        <f t="shared" si="2"/>
+        <v>2.4</v>
+      </c>
       <c r="C28" s="2">
         <v>1.776</v>
       </c>
@@ -20009,10 +20068,13 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>250</v>
       </c>
-      <c r="B29" s="2"/>
+      <c r="B29" s="2">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
       <c r="C29" s="2">
         <v>1.5529999999999999</v>
       </c>
@@ -20036,7 +20098,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="B10" activeCellId="1" sqref="B3:B8 B10:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20097,7 +20159,10 @@
       <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <f>A3/100</f>
+        <v>0</v>
+      </c>
       <c r="C3" s="2">
         <v>2.4750000000000001</v>
       </c>
@@ -20116,7 +20181,10 @@
         <f>A3+10</f>
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B24" si="0">A4/100</f>
+        <v>0.1</v>
+      </c>
       <c r="C4" s="2">
         <v>2.5249999999999999</v>
       </c>
@@ -20124,16 +20192,19 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G24" si="0">$F$2-C4</f>
+        <f t="shared" ref="G4:G24" si="1">$F$2-C4</f>
         <v>2725.232</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A8" si="1">A4+10</f>
+        <f t="shared" ref="A5:A8" si="2">A4+10</f>
         <v>20</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="C5" s="2">
         <v>2.4319999999999999</v>
       </c>
@@ -20141,16 +20212,19 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.3250000000003</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
       <c r="C6" s="2">
         <v>2.5939999999999999</v>
       </c>
@@ -20158,16 +20232,19 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.163</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
       <c r="C7" s="2">
         <v>2.629</v>
       </c>
@@ -20175,16 +20252,19 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1280000000002</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="C8" s="2">
         <v>2.653</v>
       </c>
@@ -20194,7 +20274,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1040000000003</v>
       </c>
     </row>
@@ -20202,7 +20282,10 @@
       <c r="A9" s="2">
         <v>50</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="C9" s="2">
         <v>2.419</v>
       </c>
@@ -20212,7 +20295,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.3380000000002</v>
       </c>
       <c r="H9" s="18">
@@ -20223,7 +20306,7 @@
         <v>-0.62400000000070577</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -20231,7 +20314,10 @@
         <f>A8+10</f>
         <v>60</v>
       </c>
-      <c r="B10" s="3"/>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
       <c r="C10" s="2">
         <v>2.5760000000000001</v>
       </c>
@@ -20239,7 +20325,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.181</v>
       </c>
     </row>
@@ -20248,7 +20334,10 @@
         <f>A10+10</f>
         <v>70</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
       <c r="C11" s="2">
         <v>2.6139999999999999</v>
       </c>
@@ -20256,7 +20345,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.143</v>
       </c>
       <c r="I11" s="11" t="s">
@@ -20265,10 +20354,13 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" ref="A12:A24" si="2">A11+10</f>
+        <f t="shared" ref="A12:A24" si="3">A11+10</f>
         <v>80</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
       <c r="C12" s="2">
         <v>2.6040000000000001</v>
       </c>
@@ -20276,7 +20368,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1530000000002</v>
       </c>
       <c r="I12" s="11">
@@ -20286,10 +20378,13 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
       <c r="C13" s="2">
         <v>2.6110000000000002</v>
       </c>
@@ -20297,17 +20392,20 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1460000000002</v>
       </c>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="C14" s="2">
         <v>2.6139999999999999</v>
       </c>
@@ -20315,16 +20413,19 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.143</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="B15" s="3"/>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C15" s="2">
         <v>2.5680000000000001</v>
       </c>
@@ -20332,16 +20433,19 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1889999999999</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="B16" s="3"/>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
       <c r="C16" s="2">
         <v>2.5710000000000002</v>
       </c>
@@ -20349,16 +20453,19 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1860000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
       <c r="C17" s="2">
         <v>2.601</v>
       </c>
@@ -20366,16 +20473,19 @@
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1559999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
       <c r="C18" s="2">
         <v>2.5640000000000001</v>
       </c>
@@ -20383,16 +20493,19 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1930000000002</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
       <c r="C19" s="2">
         <v>2.5609999999999999</v>
       </c>
@@ -20402,16 +20515,19 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.1959999999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
       <c r="C20" s="2">
         <v>2.496</v>
       </c>
@@ -20419,16 +20535,19 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.261</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
       <c r="C21" s="2">
         <v>2.4820000000000002</v>
       </c>
@@ -20436,16 +20555,19 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.2750000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
       <c r="C22" s="2">
         <v>2.4369999999999998</v>
       </c>
@@ -20453,16 +20575,19 @@
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.32</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
       <c r="C23" s="2">
         <v>2.3660000000000001</v>
       </c>
@@ -20470,16 +20595,19 @@
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.3910000000001</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>200</v>
       </c>
-      <c r="B24" s="3"/>
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="C24" s="2">
         <v>2.1949999999999998</v>
       </c>
@@ -20489,7 +20617,7 @@
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2725.5619999999999</v>
       </c>
     </row>
@@ -21142,7 +21270,7 @@
         <v>2733.5150000000008</v>
       </c>
       <c r="I33" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -21288,7 +21416,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B2" s="6">
         <v>2.4950000000000001</v>
@@ -21314,7 +21442,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -21428,7 +21556,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
@@ -21446,7 +21574,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
@@ -21608,7 +21736,7 @@
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
@@ -21626,7 +21754,7 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
@@ -21664,7 +21792,7 @@
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2">
@@ -21682,7 +21810,7 @@
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2">
@@ -21732,7 +21860,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
@@ -21750,7 +21878,7 @@
       </c>
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2">
@@ -21832,7 +21960,7 @@
       </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2">
@@ -21850,7 +21978,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21886,7 +22014,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B2" s="6">
         <v>2.4449999999999998</v>
@@ -21908,7 +22036,10 @@
       <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <f>A3/100</f>
+        <v>0</v>
+      </c>
       <c r="C3" s="2">
         <v>2.2450000000000001</v>
       </c>
@@ -21931,7 +22062,10 @@
         <f>A3+10</f>
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B22" si="0">A4/100</f>
+        <v>0.1</v>
+      </c>
       <c r="C4" s="2">
         <v>2.2400000000000002</v>
       </c>
@@ -21945,32 +22079,41 @@
         <v>2733.7200000000003</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H22" si="0">C4-0.5</f>
+        <f t="shared" ref="H4:H22" si="1">C4-0.5</f>
         <v>1.7400000000000002</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A11" si="1">A4+10</f>
+        <f t="shared" ref="A5:A11" si="2">A4+10</f>
         <v>20</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2.2999999999999998</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
         <v>78</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2">
+        <f t="shared" ref="G5:G22" si="3">$F$2-C5</f>
+        <v>2733.66</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
       <c r="C6" s="2">
         <v>2.4540000000000002</v>
       </c>
@@ -21978,20 +22121,23 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" ref="G6:G22" si="2">$F$2-C6</f>
+        <f t="shared" si="3"/>
         <v>2733.5059999999999</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9540000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
       <c r="C7" s="2">
         <v>2.423</v>
       </c>
@@ -21999,20 +22145,23 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.5370000000003</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.923</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="C8" s="2">
         <v>2.4470000000000001</v>
       </c>
@@ -22020,11 +22169,11 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.5129999999999</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9470000000000001</v>
       </c>
       <c r="I8" s="11" t="s">
@@ -22033,10 +22182,13 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
       <c r="C9" s="2">
         <v>2.371</v>
       </c>
@@ -22044,11 +22196,11 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.5889999999999</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.871</v>
       </c>
       <c r="I9" s="11">
@@ -22058,10 +22210,13 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
       <c r="C10" s="2">
         <v>2.3839999999999999</v>
       </c>
@@ -22069,20 +22224,23 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.576</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8839999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
       <c r="C11" s="2">
         <v>2.4140000000000001</v>
       </c>
@@ -22092,11 +22250,11 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.5459999999998</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9140000000000001</v>
       </c>
     </row>
@@ -22104,7 +22262,10 @@
       <c r="A12" s="5">
         <v>80</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
       <c r="C12" s="2">
         <v>2.2949999999999999</v>
       </c>
@@ -22114,11 +22275,11 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.665</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7949999999999999</v>
       </c>
     </row>
@@ -22127,7 +22288,10 @@
         <f>A11+10</f>
         <v>90</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
       <c r="C13" s="2">
         <v>2.476</v>
       </c>
@@ -22135,20 +22299,23 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.4839999999999</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.976</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" ref="A14:A22" si="3">A13+10</f>
+        <f t="shared" ref="A14:A22" si="4">A13+10</f>
         <v>100</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="C14" s="2">
         <v>2.5259999999999998</v>
       </c>
@@ -22156,20 +22323,23 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.4340000000002</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0259999999999998</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C15" s="2">
         <v>2.5190000000000001</v>
       </c>
@@ -22177,20 +22347,23 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.4410000000003</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0190000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
       <c r="C16" s="2">
         <v>2.387</v>
       </c>
@@ -22200,20 +22373,23 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.5729999999999</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.887</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
       <c r="C17" s="2">
         <v>2.4340000000000002</v>
       </c>
@@ -22221,20 +22397,23 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.5259999999998</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9340000000000002</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>140</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
       <c r="C18" s="2">
         <v>2.4249999999999998</v>
       </c>
@@ -22242,20 +22421,23 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.5349999999999</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9249999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>150</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
       <c r="C19" s="2">
         <v>2.3290000000000002</v>
       </c>
@@ -22263,20 +22445,23 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.6309999999999</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8290000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>160</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
       <c r="C20" s="2">
         <v>2.3149999999999999</v>
       </c>
@@ -22284,20 +22469,23 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.645</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8149999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>170</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
       <c r="C21" s="2">
         <v>2.3069999999999999</v>
       </c>
@@ -22305,20 +22493,23 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.6530000000002</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.8069999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>180</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
       <c r="C22" s="2">
         <v>2.2749999999999999</v>
       </c>
@@ -22328,11 +22519,11 @@
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2733.6849999999999</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.7749999999999999</v>
       </c>
     </row>
@@ -22346,7 +22537,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" activeCellId="1" sqref="B2:B7 B9:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22384,7 +22575,10 @@
       <c r="A2" s="6">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="6">
+        <f>A2/100</f>
+        <v>0</v>
+      </c>
       <c r="C2" s="6">
         <v>1.91</v>
       </c>
@@ -22405,7 +22599,10 @@
         <f>A2+10</f>
         <v>10</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="6">
+        <f t="shared" ref="B3:B22" si="0">A3/100</f>
+        <v>0.1</v>
+      </c>
       <c r="C3" s="2">
         <v>1.962</v>
       </c>
@@ -22415,16 +22612,19 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="6">
-        <f t="shared" ref="G3:G22" si="0">$F$2-C3</f>
+        <f t="shared" ref="G3:G22" si="1">$F$2-C3</f>
         <v>2734.0450000000001</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <f t="shared" ref="A4:A7" si="1">A3+10</f>
+        <f t="shared" ref="A4:A7" si="2">A3+10</f>
         <v>20</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="6">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="C4" s="2">
         <v>2.105</v>
       </c>
@@ -22432,16 +22632,19 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.902</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="6">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
       <c r="C5" s="2">
         <v>2.169</v>
       </c>
@@ -22449,16 +22652,19 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.8380000000002</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="6">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
       <c r="C6" s="2">
         <v>2.1549999999999998</v>
       </c>
@@ -22466,16 +22672,19 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.8519999999999</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="C7" s="2">
         <v>2.1960000000000002</v>
       </c>
@@ -22485,7 +22694,7 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.8110000000001</v>
       </c>
     </row>
@@ -22493,7 +22702,10 @@
       <c r="A8" s="2">
         <v>50</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="C8" s="2">
         <v>2.0089999999999999</v>
       </c>
@@ -22503,7 +22715,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.998</v>
       </c>
     </row>
@@ -22512,7 +22724,10 @@
         <f>A7+10</f>
         <v>60</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="6">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
       <c r="C9" s="2">
         <v>2.1560000000000001</v>
       </c>
@@ -22520,7 +22735,7 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.8510000000001</v>
       </c>
     </row>
@@ -22529,7 +22744,10 @@
         <f>A9+10</f>
         <v>70</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
       <c r="C10" s="2">
         <v>2.194</v>
       </c>
@@ -22537,7 +22755,7 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.8130000000001</v>
       </c>
       <c r="I10" s="5">
@@ -22547,10 +22765,13 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" ref="A11:A22" si="2">A10+10</f>
+        <f t="shared" ref="A11:A22" si="3">A10+10</f>
         <v>80</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="6">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
       <c r="C11" s="2">
         <v>2.2400000000000002</v>
       </c>
@@ -22558,16 +22779,19 @@
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.7670000000003</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>90</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="6">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
       <c r="C12" s="2">
         <v>2.2250000000000001</v>
       </c>
@@ -22575,16 +22799,19 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.7820000000002</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="C13" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -22592,16 +22819,19 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.8070000000002</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="6">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C14" s="2">
         <v>1.9450000000000001</v>
       </c>
@@ -22611,16 +22841,19 @@
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2734.0619999999999</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="6">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
       <c r="C15" s="2">
         <v>2.274</v>
       </c>
@@ -22628,16 +22861,19 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.7330000000002</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="6">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
       <c r="C16" s="2">
         <v>2.052</v>
       </c>
@@ -22647,16 +22883,19 @@
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2733.9549999999999</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="6">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
       <c r="C17" s="2">
         <v>1.988</v>
       </c>
@@ -22664,16 +22903,19 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2734.0190000000002</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
       <c r="C18" s="2">
         <v>1.9610000000000001</v>
       </c>
@@ -22681,16 +22923,19 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2734.0460000000003</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="6">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
       <c r="C19" s="2">
         <v>1.82</v>
       </c>
@@ -22698,16 +22943,19 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2734.1869999999999</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="6">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
       <c r="C20" s="2">
         <v>1.79</v>
       </c>
@@ -22715,16 +22963,19 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2734.2170000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="6">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
       <c r="C21" s="2">
         <v>1.7110000000000001</v>
       </c>
@@ -22732,16 +22983,19 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2734.2960000000003</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9</v>
+      </c>
       <c r="C22" s="2">
         <v>1.613</v>
       </c>
@@ -22751,7 +23005,7 @@
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2734.3940000000002</v>
       </c>
     </row>
@@ -24335,7 +24589,7 @@
         <v>2721.7620000000002</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J17">
         <f>H17-G17</f>
@@ -24602,7 +24856,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24661,7 +24915,10 @@
       <c r="A3" s="2">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2">
+        <f>A3/100</f>
+        <v>0</v>
+      </c>
       <c r="C3" s="2">
         <v>2.0379999999999998</v>
       </c>
@@ -24680,7 +24937,10 @@
         <f>A3+10</f>
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B23" si="0">A4/100</f>
+        <v>0.1</v>
+      </c>
       <c r="C4" s="2">
         <v>2.1070000000000002</v>
       </c>
@@ -24690,16 +24950,19 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
-        <f t="shared" ref="G4:G23" si="0">$F$2-C4</f>
+        <f t="shared" ref="G4:G23" si="1">$F$2-C4</f>
         <v>2735.4860000000003</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A7" si="1">A4+10</f>
+        <f t="shared" ref="A5:A7" si="2">A4+10</f>
         <v>20</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
       <c r="C5" s="2">
         <v>2.1320000000000001</v>
       </c>
@@ -24707,16 +24970,19 @@
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4610000000002</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
       <c r="C6" s="2">
         <v>2.145</v>
       </c>
@@ -24724,16 +24990,19 @@
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4480000000003</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
       <c r="C7" s="2">
         <v>2.1749999999999998</v>
       </c>
@@ -24743,7 +25012,7 @@
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4180000000001</v>
       </c>
     </row>
@@ -24751,7 +25020,10 @@
       <c r="A8" s="2">
         <v>45</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
       <c r="C8" s="2">
         <v>2.036</v>
       </c>
@@ -24761,7 +25033,7 @@
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.5570000000002</v>
       </c>
     </row>
@@ -24770,7 +25042,10 @@
         <f>A7+10</f>
         <v>50</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="C9" s="2">
         <v>2.1709999999999998</v>
       </c>
@@ -24780,7 +25055,7 @@
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4220000000005</v>
       </c>
       <c r="I9">
@@ -24793,7 +25068,10 @@
         <f>A9+10</f>
         <v>60</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
       <c r="C10" s="2">
         <v>2.2210000000000001</v>
       </c>
@@ -24803,7 +25081,7 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.3720000000003</v>
       </c>
     </row>
@@ -24811,7 +25089,10 @@
       <c r="A11" s="2">
         <v>60</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
       <c r="C11" s="2">
         <v>1.9239999999999999</v>
       </c>
@@ -24821,7 +25102,7 @@
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.6690000000003</v>
       </c>
     </row>
@@ -24830,7 +25111,10 @@
         <f>A10+10</f>
         <v>70</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
       <c r="C12" s="2">
         <v>2.1419999999999999</v>
       </c>
@@ -24838,7 +25122,7 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4510000000005</v>
       </c>
     </row>
@@ -24847,7 +25131,10 @@
         <f>A12+10</f>
         <v>80</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
       <c r="C13" s="2">
         <v>2.19</v>
       </c>
@@ -24855,7 +25142,7 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4030000000002</v>
       </c>
     </row>
@@ -24864,7 +25151,10 @@
         <f>A13+10</f>
         <v>90</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
       <c r="C14" s="2">
         <v>2.0659999999999998</v>
       </c>
@@ -24872,16 +25162,19 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.5270000000005</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" ref="A15:A23" si="2">A14+10</f>
+        <f t="shared" ref="A15:A23" si="3">A14+10</f>
         <v>100</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
       <c r="C15" s="2">
         <v>2.1259999999999999</v>
       </c>
@@ -24889,16 +25182,19 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4670000000001</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C16" s="2">
         <v>2.1230000000000002</v>
       </c>
@@ -24906,16 +25202,19 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.4700000000003</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>120</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
       <c r="C17" s="2">
         <v>2.0550000000000002</v>
       </c>
@@ -24925,16 +25224,19 @@
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.5380000000005</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>130</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
       <c r="C18" s="2">
         <v>1.8440000000000001</v>
       </c>
@@ -24942,16 +25244,19 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.7490000000003</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>140</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>1.4</v>
+      </c>
       <c r="C19" s="2">
         <v>1.784</v>
       </c>
@@ -24959,16 +25264,19 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.8090000000002</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
       <c r="C20" s="2">
         <v>1.69</v>
       </c>
@@ -24976,16 +25284,19 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.9030000000002</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>160</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
       <c r="C21" s="2">
         <v>1.641</v>
       </c>
@@ -24993,16 +25304,19 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.9520000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>170</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
       <c r="C22" s="2">
         <v>1.595</v>
       </c>
@@ -25010,16 +25324,19 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.9980000000005</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>180</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
       <c r="C23" s="2">
         <v>1.665</v>
       </c>
@@ -25029,7 +25346,7 @@
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2735.9280000000003</v>
       </c>
     </row>
@@ -26501,7 +26818,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="6">
         <v>2.8149999999999999</v>
@@ -26522,7 +26839,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="2">
         <v>2.4449999999999998</v>
@@ -26550,7 +26867,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2">
@@ -26616,7 +26933,7 @@
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2">
@@ -26714,7 +27031,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
@@ -26732,7 +27049,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
@@ -26946,7 +27263,7 @@
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2">
@@ -27091,8 +27408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46C12D5E-274C-49F4-AC1E-9E3A5CF8DFEE}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27128,7 +27445,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B2" s="2">
         <v>2.4449999999999998</v>
@@ -27138,7 +27455,7 @@
         <v>0.7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F2" s="2">
         <f>G2+B2</f>
@@ -27158,7 +27475,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2">
@@ -27352,7 +27669,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2">
@@ -27370,7 +27687,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2">
@@ -27615,8 +27932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15857BB-7009-42F0-BB33-F587ED47BBA2}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27698,7 +28015,7 @@
         <v>2737.4559999999997</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L2" s="2">
         <v>3.165</v>
@@ -27764,6 +28081,9 @@
         <f t="shared" ref="G4:G26" si="0">$F$2-C4</f>
         <v>2738.4929999999995</v>
       </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
       <c r="K4" s="2" t="s">
         <v>133</v>
       </c>
@@ -27795,6 +28115,9 @@
         <f t="shared" si="0"/>
         <v>2738.3429999999994</v>
       </c>
+      <c r="J5">
+        <v>0.1</v>
+      </c>
       <c r="K5" s="2" t="s">
         <v>134</v>
       </c>
@@ -27826,6 +28149,10 @@
         <f t="shared" si="0"/>
         <v>2738.2829999999994</v>
       </c>
+      <c r="J6">
+        <f>K6-1</f>
+        <v>0.19999999999999996</v>
+      </c>
       <c r="K6" s="2">
         <v>1.2</v>
       </c>
@@ -27857,6 +28184,10 @@
         <f t="shared" si="0"/>
         <v>2738.2769999999996</v>
       </c>
+      <c r="J7">
+        <f t="shared" ref="J7:J29" si="3">K7-1</f>
+        <v>0.30000000000000004</v>
+      </c>
       <c r="K7" s="2">
         <v>1.3</v>
       </c>
@@ -27890,6 +28221,10 @@
         <f t="shared" si="0"/>
         <v>2738.2569999999996</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>0.39999999999999991</v>
+      </c>
       <c r="K8" s="2">
         <v>1.4</v>
       </c>
@@ -27924,6 +28259,10 @@
       <c r="I9" s="11" t="s">
         <v>117</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
       <c r="K9" s="2">
         <v>1.5</v>
       </c>
@@ -27959,6 +28298,10 @@
         <f>C20-C21</f>
         <v>0.248</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="3"/>
+        <v>0.60000000000000009</v>
+      </c>
       <c r="K10" s="2">
         <v>1.6</v>
       </c>
@@ -27991,6 +28334,10 @@
       <c r="G11" s="6">
         <f t="shared" si="0"/>
         <v>2738.2519999999995</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
       </c>
       <c r="K11" s="2">
         <v>1.7</v>
@@ -28026,6 +28373,10 @@
       <c r="I12" s="11" t="s">
         <v>130</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
+      </c>
       <c r="K12" s="2">
         <v>1.8</v>
       </c>
@@ -28062,6 +28413,10 @@
       <c r="I13" s="11">
         <f>M17-M18</f>
         <v>0.19300000000000006</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="3"/>
+        <v>0.89999999999999991</v>
       </c>
       <c r="K13" s="2">
         <v>1.9</v>
@@ -28096,6 +28451,10 @@
         <f t="shared" si="0"/>
         <v>2738.4449999999993</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="K14" s="2">
         <v>2</v>
       </c>
@@ -28127,6 +28486,10 @@
         <f t="shared" si="0"/>
         <v>2738.4119999999994</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="K15" s="2">
         <v>2.1</v>
       </c>
@@ -28158,6 +28521,10 @@
         <f t="shared" si="0"/>
         <v>2738.3989999999994</v>
       </c>
+      <c r="J16">
+        <f t="shared" si="3"/>
+        <v>1.2000000000000002</v>
+      </c>
       <c r="K16" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -28189,6 +28556,10 @@
         <f t="shared" si="0"/>
         <v>2738.3309999999997</v>
       </c>
+      <c r="J17">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
       <c r="K17" s="2">
         <v>2.25</v>
       </c>
@@ -28222,6 +28593,10 @@
         <f t="shared" si="0"/>
         <v>2738.3119999999994</v>
       </c>
+      <c r="J18">
+        <f t="shared" si="3"/>
+        <v>1.25</v>
+      </c>
       <c r="K18" s="2">
         <v>2.25</v>
       </c>
@@ -28254,6 +28629,10 @@
       <c r="G19" s="6">
         <f t="shared" si="0"/>
         <v>2738.2349999999997</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="3"/>
+        <v>1.2999999999999998</v>
       </c>
       <c r="K19" s="2">
         <v>2.2999999999999998</v>
@@ -28288,6 +28667,10 @@
         <f t="shared" si="0"/>
         <v>2738.2259999999997</v>
       </c>
+      <c r="J20">
+        <f t="shared" si="3"/>
+        <v>1.4</v>
+      </c>
       <c r="K20" s="2">
         <v>2.4</v>
       </c>
@@ -28321,6 +28704,10 @@
       <c r="G21" s="6">
         <f t="shared" si="0"/>
         <v>2738.4739999999997</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="3"/>
+        <v>1.5</v>
       </c>
       <c r="K21" s="2">
         <v>2.5</v>
@@ -28355,6 +28742,10 @@
         <f t="shared" si="0"/>
         <v>2738.2919999999995</v>
       </c>
+      <c r="J22">
+        <f t="shared" si="3"/>
+        <v>1.6</v>
+      </c>
       <c r="K22" s="2">
         <v>2.6</v>
       </c>
@@ -28386,6 +28777,10 @@
         <f t="shared" si="0"/>
         <v>2738.4159999999993</v>
       </c>
+      <c r="J23">
+        <f t="shared" si="3"/>
+        <v>1.7000000000000002</v>
+      </c>
       <c r="K23" s="2">
         <v>2.7</v>
       </c>
@@ -28417,6 +28812,10 @@
         <f t="shared" si="0"/>
         <v>2738.4679999999994</v>
       </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>1.7999999999999998</v>
+      </c>
       <c r="K24" s="2">
         <v>2.8</v>
       </c>
@@ -28448,6 +28847,10 @@
         <f t="shared" si="0"/>
         <v>2738.4629999999993</v>
       </c>
+      <c r="J25">
+        <f t="shared" si="3"/>
+        <v>1.9</v>
+      </c>
       <c r="K25" s="2">
         <v>2.9</v>
       </c>
@@ -28483,8 +28886,12 @@
         <f t="shared" si="0"/>
         <v>2738.4569999999994</v>
       </c>
-      <c r="K26" s="2" t="s">
-        <v>137</v>
+      <c r="J26">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="K26" s="2">
+        <v>3</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="2">
@@ -28504,6 +28911,10 @@
       </c>
       <c r="D27" s="24"/>
       <c r="E27" s="24"/>
+      <c r="J27">
+        <f t="shared" si="3"/>
+        <v>2.1</v>
+      </c>
       <c r="K27" s="2">
         <v>3.1</v>
       </c>
@@ -28513,7 +28924,7 @@
       </c>
       <c r="N27" s="2"/>
       <c r="O27" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P27" s="3"/>
       <c r="Q27" s="2">
@@ -28522,6 +28933,10 @@
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000002</v>
+      </c>
       <c r="K28" s="2">
         <v>3.2</v>
       </c>
@@ -28531,7 +28946,7 @@
       </c>
       <c r="N28" s="2"/>
       <c r="O28" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="2">
@@ -28540,6 +28955,10 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <f t="shared" si="3"/>
+        <v>2.2999999999999998</v>
+      </c>
       <c r="K29" s="2">
         <v>3.3</v>
       </c>
@@ -28549,7 +28968,7 @@
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="P29" s="3"/>
       <c r="Q29" s="2">
@@ -29598,7 +30017,7 @@
         <v>2722.52</v>
       </c>
       <c r="I10" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J10" s="5">
         <f>H10-G10</f>
@@ -30396,7 +30815,7 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="O9" sqref="J9:O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30421,7 +30840,7 @@
       <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
@@ -30463,7 +30882,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="6"/>
-      <c r="C2" s="2">
+      <c r="C2" s="6">
         <v>3.3260000000000001</v>
       </c>
       <c r="D2" s="6"/>
@@ -30545,6 +30964,10 @@
         <f t="shared" si="0"/>
         <v>2722.5989999999997</v>
       </c>
+      <c r="J4" s="22">
+        <f>K4/100</f>
+        <v>0.1</v>
+      </c>
       <c r="K4" s="2">
         <v>10</v>
       </c>
@@ -30578,6 +31001,10 @@
         <f t="shared" si="0"/>
         <v>2722.5309999999999</v>
       </c>
+      <c r="J5" s="22">
+        <f t="shared" ref="J5:J24" si="3">K5/100</f>
+        <v>0.2</v>
+      </c>
       <c r="K5" s="2">
         <v>20</v>
       </c>
@@ -30609,6 +31036,10 @@
         <f t="shared" si="0"/>
         <v>2722.5299999999997</v>
       </c>
+      <c r="J6" s="22">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
       <c r="K6" s="2">
         <v>30</v>
       </c>
@@ -30640,6 +31071,10 @@
         <f t="shared" si="0"/>
         <v>2722.5149999999999</v>
       </c>
+      <c r="J7" s="22">
+        <f t="shared" si="3"/>
+        <v>0.4</v>
+      </c>
       <c r="K7" s="2">
         <v>40</v>
       </c>
@@ -30671,6 +31106,10 @@
         <f t="shared" si="0"/>
         <v>2722.4839999999999</v>
       </c>
+      <c r="J8" s="22">
+        <f t="shared" si="3"/>
+        <v>0.5</v>
+      </c>
       <c r="K8" s="2">
         <v>50</v>
       </c>
@@ -30702,6 +31141,10 @@
         <f t="shared" si="0"/>
         <v>2722.5140000000001</v>
       </c>
+      <c r="J9" s="22">
+        <f t="shared" si="3"/>
+        <v>0.6</v>
+      </c>
       <c r="K9" s="2">
         <v>60</v>
       </c>
@@ -30720,7 +31163,7 @@
       </c>
       <c r="R9" s="5"/>
       <c r="S9" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -30739,6 +31182,10 @@
         <f t="shared" si="0"/>
         <v>2722.509</v>
       </c>
+      <c r="J10" s="22">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
       <c r="K10" s="2">
         <v>70</v>
       </c>
@@ -30779,6 +31226,10 @@
         <f t="shared" si="0"/>
         <v>2722.5009999999997</v>
       </c>
+      <c r="J11" s="22">
+        <f t="shared" si="3"/>
+        <v>0.7</v>
+      </c>
       <c r="K11" s="2">
         <v>70</v>
       </c>
@@ -30811,6 +31262,10 @@
       <c r="G12" s="6">
         <f t="shared" si="0"/>
         <v>2722.0859999999998</v>
+      </c>
+      <c r="J12" s="22">
+        <f t="shared" si="3"/>
+        <v>0.8</v>
       </c>
       <c r="K12" s="2">
         <v>80</v>
@@ -30843,6 +31298,10 @@
       <c r="I13" s="11" t="s">
         <v>116</v>
       </c>
+      <c r="J13" s="22">
+        <f t="shared" si="3"/>
+        <v>0.9</v>
+      </c>
       <c r="K13" s="2">
         <v>90</v>
       </c>
@@ -30880,6 +31339,10 @@
         <f>G15-G14</f>
         <v>0.13900000000012369</v>
       </c>
+      <c r="J14" s="22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
       <c r="K14" s="2">
         <v>100</v>
       </c>
@@ -30909,8 +31372,12 @@
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="6">
-        <f t="shared" ref="G15:G31" si="3">$F$2-C15</f>
+        <f t="shared" ref="G15:G31" si="4">$F$2-C15</f>
         <v>2722.652</v>
+      </c>
+      <c r="J15" s="22">
+        <f t="shared" si="3"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K15" s="2">
         <v>110</v>
@@ -30940,11 +31407,15 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.49</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>130</v>
+      </c>
+      <c r="J16" s="22">
+        <f t="shared" si="3"/>
+        <v>1.2</v>
       </c>
       <c r="K16" s="2">
         <v>120</v>
@@ -30963,7 +31434,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" ref="A17:A31" si="4">A16+10</f>
+        <f t="shared" ref="A17:A31" si="5">A16+10</f>
         <v>140</v>
       </c>
       <c r="B17" s="2"/>
@@ -30974,12 +31445,16 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.491</v>
       </c>
       <c r="I17" s="11">
         <f>M10-M11</f>
         <v>0.19399999999999995</v>
+      </c>
+      <c r="J17" s="22">
+        <f t="shared" si="3"/>
+        <v>1.3</v>
       </c>
       <c r="K17" s="2">
         <v>130</v>
@@ -31000,7 +31475,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
       <c r="B18" s="2"/>
@@ -31011,8 +31486,12 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="6">
+        <f t="shared" si="4"/>
+        <v>2722.502</v>
+      </c>
+      <c r="J18" s="22">
         <f t="shared" si="3"/>
-        <v>2722.502</v>
+        <v>1.4</v>
       </c>
       <c r="K18" s="2">
         <v>140</v>
@@ -31031,7 +31510,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
       <c r="B19" s="2"/>
@@ -31042,8 +31521,12 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="6">
+        <f t="shared" si="4"/>
+        <v>2722.5299999999997</v>
+      </c>
+      <c r="J19" s="22">
         <f t="shared" si="3"/>
-        <v>2722.5299999999997</v>
+        <v>1.5</v>
       </c>
       <c r="K19" s="2">
         <v>150</v>
@@ -31062,7 +31545,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
       <c r="B20" s="2"/>
@@ -31075,8 +31558,12 @@
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="6">
+        <f t="shared" si="4"/>
+        <v>2722.5319999999997</v>
+      </c>
+      <c r="J20" s="22">
         <f t="shared" si="3"/>
-        <v>2722.5319999999997</v>
+        <v>1.6</v>
       </c>
       <c r="K20" s="2">
         <v>160</v>
@@ -31095,7 +31582,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
       <c r="B21" s="2"/>
@@ -31106,8 +31593,12 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="6">
+        <f t="shared" si="4"/>
+        <v>2722.558</v>
+      </c>
+      <c r="J21" s="22">
         <f t="shared" si="3"/>
-        <v>2722.558</v>
+        <v>1.7</v>
       </c>
       <c r="K21" s="2">
         <v>170</v>
@@ -31126,7 +31617,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
       <c r="B22" s="2"/>
@@ -31137,8 +31628,12 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="6">
+        <f t="shared" si="4"/>
+        <v>2722.5569999999998</v>
+      </c>
+      <c r="J22" s="22">
         <f t="shared" si="3"/>
-        <v>2722.5569999999998</v>
+        <v>1.8</v>
       </c>
       <c r="K22" s="2">
         <v>180</v>
@@ -31157,7 +31652,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
       <c r="B23" s="2"/>
@@ -31168,8 +31663,12 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="6">
+        <f t="shared" si="4"/>
+        <v>2722.5909999999999</v>
+      </c>
+      <c r="J23" s="22">
         <f t="shared" si="3"/>
-        <v>2722.5909999999999</v>
+        <v>1.9</v>
       </c>
       <c r="K23" s="2">
         <v>190</v>
@@ -31188,7 +31687,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>210</v>
       </c>
       <c r="B24" s="2"/>
@@ -31199,8 +31698,12 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="6">
+        <f t="shared" si="4"/>
+        <v>2722.5720000000001</v>
+      </c>
+      <c r="J24" s="22">
         <f t="shared" si="3"/>
-        <v>2722.5720000000001</v>
+        <v>2</v>
       </c>
       <c r="K24" s="2">
         <v>200</v>
@@ -31219,7 +31722,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>220</v>
       </c>
       <c r="B25" s="2"/>
@@ -31230,13 +31733,13 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.578</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>230</v>
       </c>
       <c r="B26" s="2"/>
@@ -31247,7 +31750,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.5949999999998</v>
       </c>
       <c r="K26" s="24" t="s">
@@ -31262,7 +31765,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>240</v>
       </c>
       <c r="B27" s="2"/>
@@ -31273,14 +31776,14 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.605</v>
       </c>
       <c r="O27" s="23"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>250</v>
       </c>
       <c r="B28" s="2"/>
@@ -31293,14 +31796,14 @@
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.8269999999998</v>
       </c>
       <c r="O28" s="23"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>260</v>
       </c>
       <c r="B29" s="2"/>
@@ -31311,14 +31814,14 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.8319999999999</v>
       </c>
       <c r="O29" s="23"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>270</v>
       </c>
       <c r="B30" s="2"/>
@@ -31329,14 +31832,14 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.8669999999997</v>
       </c>
       <c r="O30" s="23"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>280</v>
       </c>
       <c r="B31" s="2"/>
@@ -31349,7 +31852,7 @@
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2722.9139999999998</v>
       </c>
     </row>
@@ -31389,7 +31892,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>1</v>
@@ -32163,7 +32666,7 @@
         <v>2723.0129999999999</v>
       </c>
       <c r="I8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -32599,7 +33102,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32695,7 +33198,10 @@
         <f>A3+10</f>
         <v>10</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <f>A4/100</f>
+        <v>0.1</v>
+      </c>
       <c r="C4" s="2">
         <v>2.5390000000000001</v>
       </c>
@@ -32718,7 +33224,10 @@
         <f t="shared" ref="A5:A11" si="1">A4+10</f>
         <v>20</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <f t="shared" ref="B5:B25" si="2">A5/100</f>
+        <v>0.2</v>
+      </c>
       <c r="C5" s="2">
         <v>2.597</v>
       </c>
@@ -32743,7 +33252,10 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
       <c r="C6" s="2">
         <v>2.6379999999999999</v>
       </c>
@@ -32766,7 +33278,10 @@
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
       <c r="C7" s="2">
         <v>2.6339999999999999</v>
       </c>
@@ -32789,7 +33304,10 @@
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
       <c r="C8" s="2">
         <v>2.645</v>
       </c>
@@ -32812,7 +33330,10 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
       <c r="C9" s="2">
         <v>2.6549999999999998</v>
       </c>
@@ -32839,7 +33360,10 @@
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
       <c r="C10" s="2">
         <v>2.6560000000000001</v>
       </c>
@@ -32858,7 +33382,7 @@
         <v>2.5390000000000001</v>
       </c>
       <c r="T10" s="2">
-        <f t="shared" ref="T10:T31" si="2">$U$3-S10</f>
+        <f t="shared" ref="T10:T31" si="3">$U$3-S10</f>
         <v>7.4610000000000003</v>
       </c>
     </row>
@@ -32867,7 +33391,10 @@
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
       <c r="C11" s="2">
         <v>2.649</v>
       </c>
@@ -32888,14 +33415,14 @@
         <v>3.9999999989959178E-3</v>
       </c>
       <c r="R11" s="2">
-        <f t="shared" ref="R11:R17" si="3">R10+10</f>
+        <f t="shared" ref="R11:R17" si="4">R10+10</f>
         <v>20</v>
       </c>
       <c r="S11" s="2">
         <v>2.597</v>
       </c>
       <c r="T11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4030000000000005</v>
       </c>
     </row>
@@ -32903,7 +33430,10 @@
       <c r="A12" s="2">
         <v>80</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
       <c r="C12" s="2">
         <v>2.4449999999999998</v>
       </c>
@@ -32917,14 +33447,14 @@
         <v>2723.3890000000001</v>
       </c>
       <c r="R12" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="S12" s="2">
         <v>2.6379999999999999</v>
       </c>
       <c r="T12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3620000000000001</v>
       </c>
     </row>
@@ -32933,63 +33463,72 @@
         <f>A11+10</f>
         <v>90</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="2">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
       <c r="C13" s="2">
-        <v>2.5369999999999999</v>
+        <v>2.637</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2">
         <f t="shared" si="0"/>
-        <v>2723.2970000000005</v>
+        <v>2723.1970000000001</v>
       </c>
       <c r="R13" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="S13" s="2">
         <v>2.6339999999999999</v>
       </c>
       <c r="T13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3659999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" ref="A14:A26" si="4">A13+10</f>
+        <f t="shared" ref="A14:A26" si="5">A13+10</f>
         <v>100</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
       <c r="C14" s="2">
-        <v>2.5750000000000002</v>
+        <v>2.6749999999999998</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>2723.2590000000005</v>
+        <v>2723.1590000000001</v>
       </c>
       <c r="R14" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="S14" s="2">
         <v>2.645</v>
       </c>
       <c r="T14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3550000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>110</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000001</v>
+      </c>
       <c r="C15" s="2">
         <v>2.6709999999999998</v>
       </c>
@@ -33001,23 +33540,26 @@
         <v>2723.1630000000005</v>
       </c>
       <c r="R15" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="S15" s="2">
         <v>2.6549999999999998</v>
       </c>
       <c r="T15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3450000000000006</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>120</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
       <c r="C16" s="2">
         <v>2.6360000000000001</v>
       </c>
@@ -33029,23 +33571,26 @@
         <v>2723.1980000000003</v>
       </c>
       <c r="R16" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="S16" s="2">
         <v>2.6560000000000001</v>
       </c>
       <c r="T16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3439999999999994</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>130</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <f t="shared" si="2"/>
+        <v>1.3</v>
+      </c>
       <c r="C17" s="2">
         <v>2.6139999999999999</v>
       </c>
@@ -33057,23 +33602,26 @@
         <v>2723.2200000000003</v>
       </c>
       <c r="R17" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="S17" s="2">
         <v>2.649</v>
       </c>
       <c r="T17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.351</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
       <c r="C18" s="2">
         <v>2.653</v>
       </c>
@@ -33092,16 +33640,19 @@
         <v>2.5369999999999999</v>
       </c>
       <c r="T18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4630000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>150</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
       <c r="C19" s="2">
         <v>2.609</v>
       </c>
@@ -33113,23 +33664,26 @@
         <v>2723.2250000000004</v>
       </c>
       <c r="R19" s="2">
-        <f t="shared" ref="R19:R31" si="5">R18+10</f>
+        <f t="shared" ref="R19:R31" si="6">R18+10</f>
         <v>100</v>
       </c>
       <c r="S19" s="2">
         <v>2.5750000000000002</v>
       </c>
       <c r="T19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4249999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>160</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
       <c r="C20" s="2">
         <v>2.6139999999999999</v>
       </c>
@@ -33141,23 +33695,26 @@
         <v>2723.2200000000003</v>
       </c>
       <c r="R20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>110</v>
       </c>
       <c r="S20" s="2">
         <v>2.6709999999999998</v>
       </c>
       <c r="T20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3290000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7</v>
+      </c>
       <c r="C21" s="2">
         <v>2.5840000000000001</v>
       </c>
@@ -33171,23 +33728,26 @@
         <v>2723.2500000000005</v>
       </c>
       <c r="R21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>120</v>
       </c>
       <c r="S21" s="2">
         <v>2.6360000000000001</v>
       </c>
       <c r="T21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3639999999999999</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>180</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8</v>
+      </c>
       <c r="C22" s="2">
         <v>2.4889999999999999</v>
       </c>
@@ -33202,23 +33762,26 @@
         <v>117</v>
       </c>
       <c r="R22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>130</v>
       </c>
       <c r="S22" s="2">
         <v>2.6139999999999999</v>
       </c>
       <c r="T22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3860000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>190</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9</v>
+      </c>
       <c r="C23" s="2">
         <v>2.4580000000000002</v>
       </c>
@@ -33234,23 +33797,26 @@
         <v>0.20400000000000018</v>
       </c>
       <c r="R23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>140</v>
       </c>
       <c r="S23" s="2">
         <v>2.653</v>
       </c>
       <c r="T23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3469999999999995</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>200</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="C24" s="2">
         <v>2.3969999999999998</v>
       </c>
@@ -33262,23 +33828,26 @@
         <v>2723.4370000000004</v>
       </c>
       <c r="R24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>150</v>
       </c>
       <c r="S24" s="2">
         <v>2.609</v>
       </c>
       <c r="T24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.391</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>210</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2">
+        <f t="shared" si="2"/>
+        <v>2.1</v>
+      </c>
       <c r="C25" s="2">
         <v>2.2829999999999999</v>
       </c>
@@ -33290,23 +33859,26 @@
         <v>2723.5510000000004</v>
       </c>
       <c r="R25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>160</v>
       </c>
       <c r="S25" s="2">
         <v>2.6139999999999999</v>
       </c>
       <c r="T25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.3860000000000001</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>220</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2">
+        <f>A26/100</f>
+        <v>2.2000000000000002</v>
+      </c>
       <c r="C26" s="2">
         <v>2.1840000000000002</v>
       </c>
@@ -33320,79 +33892,79 @@
         <v>2723.65</v>
       </c>
       <c r="R26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>170</v>
       </c>
       <c r="S26" s="2">
         <v>2.5840000000000001</v>
       </c>
       <c r="T26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.4160000000000004</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="R27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>180</v>
       </c>
       <c r="S27" s="2">
         <v>2.4889999999999999</v>
       </c>
       <c r="T27" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5110000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="R28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>190</v>
       </c>
       <c r="S28" s="2">
         <v>2.4580000000000002</v>
       </c>
       <c r="T28" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.5419999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="R29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>200</v>
       </c>
       <c r="S29" s="2">
         <v>2.3969999999999998</v>
       </c>
       <c r="T29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.6029999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="R30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>210</v>
       </c>
       <c r="S30" s="2">
         <v>2.2829999999999999</v>
       </c>
       <c r="T30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.7170000000000005</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="R31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>220</v>
       </c>
       <c r="S31" s="2">
         <v>2.1840000000000002</v>
       </c>
       <c r="T31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.8159999999999998</v>
       </c>
     </row>

</xml_diff>

<commit_message>
calculated average depth of top hyporheic layer
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
+++ b/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A3082D-E847-4C25-AD8B-4B69B0E1B242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1F22C1-07B0-406B-A853-BF594DA55365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24135" yWindow="315" windowWidth="22260" windowHeight="14940" tabRatio="804" firstSheet="12" activeTab="24" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" tabRatio="804" firstSheet="9" activeTab="24" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
   </bookViews>
   <sheets>
     <sheet name="Piezo 1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="167">
   <si>
     <t>Distance</t>
   </si>
@@ -553,6 +553,12 @@
   </si>
   <si>
     <t>top piezo 6 c</t>
+  </si>
+  <si>
+    <t>avg t probe layer depth</t>
+  </si>
+  <si>
+    <t>median</t>
   </si>
 </sst>
 </file>
@@ -19468,7 +19474,7 @@
   <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19773,6 +19779,10 @@
         <f t="shared" si="0"/>
         <v>2724.7089999999998</v>
       </c>
+      <c r="I14">
+        <f>0.4-I12</f>
+        <v>0.17499999999999993</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -20098,7 +20108,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" activeCellId="1" sqref="B3:B8 B10:B24"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20415,6 +20425,10 @@
       <c r="G14" s="2">
         <f t="shared" si="1"/>
         <v>2725.143</v>
+      </c>
+      <c r="I14">
+        <f>0.4-I12</f>
+        <v>0.16600000000000004</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -21975,10 +21989,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1C4FEB0-1102-4DB7-BB00-AF8A05932E4C}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21989,7 +22003,7 @@
     <col min="7" max="7" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -22012,7 +22026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>144</v>
       </c>
@@ -22032,7 +22046,7 @@
         <v>2733.5149999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -22057,7 +22071,7 @@
         <v>1.7450000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A3+10</f>
         <v>10</v>
@@ -22083,7 +22097,7 @@
         <v>1.7400000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A11" si="2">A4+10</f>
         <v>20</v>
@@ -22105,7 +22119,7 @@
         <v>2733.66</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -22129,7 +22143,7 @@
         <v>1.9540000000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -22153,7 +22167,7 @@
         <v>1.923</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
@@ -22180,7 +22194,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="2"/>
         <v>60</v>
@@ -22208,7 +22222,7 @@
         <v>0.11900000000000022</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="2"/>
         <v>70</v>
@@ -22232,7 +22246,7 @@
         <v>1.8839999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="2"/>
         <v>80</v>
@@ -22258,7 +22272,7 @@
         <v>1.9140000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>80</v>
       </c>
@@ -22283,7 +22297,7 @@
         <v>1.7949999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f>A11+10</f>
         <v>90</v>
@@ -22307,7 +22321,7 @@
         <v>1.976</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" ref="A14:A22" si="4">A13+10</f>
         <v>100</v>
@@ -22330,8 +22344,12 @@
         <f t="shared" si="1"/>
         <v>2.0259999999999998</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <f>0.4-I9</f>
+        <v>0.28099999999999981</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="4"/>
         <v>110</v>
@@ -22355,7 +22373,7 @@
         <v>2.0190000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="4"/>
         <v>120</v>
@@ -22537,7 +22555,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" activeCellId="1" sqref="B2:B7 B9:B22"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22801,6 +22819,10 @@
       <c r="G12" s="6">
         <f t="shared" si="1"/>
         <v>2733.7820000000002</v>
+      </c>
+      <c r="I12">
+        <f>0.4-I10</f>
+        <v>0.21299999999999975</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -24856,7 +24878,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25104,6 +25126,10 @@
       <c r="G11" s="2">
         <f t="shared" si="1"/>
         <v>2735.6690000000003</v>
+      </c>
+      <c r="I11">
+        <f>0.4-I9</f>
+        <v>0.10299999999999987</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -27930,10 +27956,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15857BB-7009-42F0-BB33-F587ED47BBA2}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28521,6 +28547,10 @@
         <f t="shared" si="0"/>
         <v>2738.3989999999994</v>
       </c>
+      <c r="I16">
+        <f>0.4-I13</f>
+        <v>0.20699999999999996</v>
+      </c>
       <c r="J16">
         <f t="shared" si="3"/>
         <v>1.2000000000000002</v>
@@ -28983,6 +29013,28 @@
       <c r="M30" s="24"/>
       <c r="N30" s="24"/>
       <c r="O30" s="24"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F35" s="20">
+        <f>AVERAGE(20.6,19.6,17.5,28.1,21.3,10.3,20.7)</f>
+        <v>19.728571428571428</v>
+      </c>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F37" s="20">
+        <f>MEDIAN(20.6,19.6,17.5,28.1,21.3,10.3,20.7)</f>
+        <v>20.6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -30815,7 +30867,7 @@
   <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O9" sqref="J9:O9"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31523,6 +31575,10 @@
       <c r="G19" s="6">
         <f t="shared" si="4"/>
         <v>2722.5299999999997</v>
+      </c>
+      <c r="I19">
+        <f>0.4-I17</f>
+        <v>0.20600000000000007</v>
       </c>
       <c r="J19" s="22">
         <f t="shared" si="3"/>
@@ -33102,7 +33158,7 @@
   <dimension ref="A1:U31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33890,6 +33946,10 @@
       <c r="G26" s="2">
         <f t="shared" si="0"/>
         <v>2723.65</v>
+      </c>
+      <c r="J26">
+        <f>0.4-J23</f>
+        <v>0.19599999999999984</v>
       </c>
       <c r="R26" s="2">
         <f t="shared" si="6"/>

</xml_diff>

<commit_message>
GW tweaks for andy
added lateral distance from channel to GW in the topo file
changed the P1B timeseries column for clarity
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
+++ b/Topography/LaJara_TopoSurvey/LaJara_XS_Topography .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1F22C1-07B0-406B-A853-BF594DA55365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{685CE9E7-CAB2-4469-AAF1-95AB19FF39F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" tabRatio="804" firstSheet="9" activeTab="24" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="804" firstSheet="9" activeTab="9" xr2:uid="{24083E57-F3BF-4A8D-A2E4-8E86074BFB86}"/>
   </bookViews>
   <sheets>
     <sheet name="Piezo 1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="168">
   <si>
     <t>Distance</t>
   </si>
@@ -560,6 +560,9 @@
   <si>
     <t>median</t>
   </si>
+  <si>
+    <t>GW distance from channel</t>
+  </si>
 </sst>
 </file>
 
@@ -732,7 +735,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -789,9 +792,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -887,7 +887,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1277,7 +1277,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1680724640"/>
@@ -1339,7 +1339,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1680722144"/>
@@ -1387,7 +1387,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1919,7 +1919,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1568800591"/>
@@ -1981,7 +1981,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015223983"/>
@@ -2029,7 +2029,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2492,7 +2492,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="583681535"/>
@@ -2554,7 +2554,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811039471"/>
@@ -2602,7 +2602,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3158,7 +3158,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1701696767"/>
@@ -3220,7 +3220,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1869339711"/>
@@ -3268,7 +3268,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3815,7 +3815,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="584295391"/>
@@ -3877,7 +3877,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1869286815"/>
@@ -3925,7 +3925,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3976,7 +3976,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4279,7 +4279,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1753949856"/>
@@ -4341,7 +4341,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1753949024"/>
@@ -4389,7 +4389,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5005,7 +5005,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2043194127"/>
@@ -5067,7 +5067,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2015234655"/>
@@ -5115,7 +5115,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5764,7 +5764,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1810760255"/>
@@ -5826,7 +5826,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811056175"/>
@@ -5874,7 +5874,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6405,7 +6405,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1993662911"/>
@@ -6467,7 +6467,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811060815"/>
@@ -6515,7 +6515,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6890,7 +6890,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1273530959"/>
@@ -6953,7 +6953,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1273528463"/>
@@ -7001,7 +7001,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -7052,7 +7052,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-AR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -7470,7 +7470,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1946070992"/>
@@ -7532,7 +7532,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1645237152"/>
@@ -7580,7 +7580,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8238,7 +8238,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1988108927"/>
@@ -8300,7 +8300,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811050607"/>
@@ -8348,7 +8348,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -8859,7 +8859,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2008535167"/>
@@ -8921,7 +8921,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1811067311"/>
@@ -8969,7 +8969,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-AR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -16254,15 +16254,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>516255</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>573405</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>211455</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>268605</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16295,15 +16295,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>392431</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>116204</xdr:rowOff>
+      <xdr:colOff>276226</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>24764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>203836</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>180974</xdr:rowOff>
+      <xdr:colOff>87631</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>99059</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16377,15 +16377,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>337185</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>339090</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16885,9 +16885,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -16925,7 +16925,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -17031,7 +17031,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -17173,7 +17173,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -17801,8 +17801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCDB23-7E29-4E96-BC9F-97898B9633F1}">
   <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17839,6 +17839,9 @@
       <c r="G1" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
@@ -17858,6 +17861,10 @@
       <c r="G2" s="6">
         <f>$F$2-C2</f>
         <v>2724.1630000000005</v>
+      </c>
+      <c r="I2">
+        <f>A35-A7</f>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -20645,7 +20652,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20657,7 +20664,7 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -20679,8 +20686,11 @@
       <c r="G1" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>68</v>
       </c>
@@ -20702,8 +20712,12 @@
         <f>2727.757-D2</f>
         <v>2727.5860000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>A33-A17</f>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
@@ -20724,7 +20738,7 @@
         <v>2730.6360000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>70</v>
       </c>
@@ -20745,7 +20759,7 @@
         <v>2732.5620000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>71</v>
       </c>
@@ -20766,7 +20780,7 @@
         <v>2733.5230000000006</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>0</v>
       </c>
@@ -20787,7 +20801,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f>A6+10</f>
         <v>10</v>
@@ -20810,7 +20824,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" ref="A8:A31" si="1">A7+10</f>
         <v>20</v>
@@ -20830,7 +20844,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -20850,7 +20864,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -20870,7 +20884,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -20890,7 +20904,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -20910,7 +20924,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -20930,7 +20944,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -20950,7 +20964,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -20970,7 +20984,7 @@
         <v>2732.9305000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -23041,7 +23055,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23053,7 +23067,7 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -23075,8 +23089,11 @@
       <c r="G1" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>86</v>
       </c>
@@ -23098,8 +23115,12 @@
         <f>2736.007-D2</f>
         <v>2734.7739999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>A11- A20</f>
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>0</v>
       </c>
@@ -23117,7 +23138,7 @@
         <v>2734.8239999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f>A3+10</f>
         <v>10</v>
@@ -23134,7 +23155,7 @@
         <v>2734.8089999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" ref="A5:A10" si="1">A4+10</f>
         <v>20</v>
@@ -23151,7 +23172,7 @@
         <v>2734.8419999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -23168,7 +23189,7 @@
         <v>2734.7749999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -23185,7 +23206,7 @@
         <v>2734.7709999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -23202,7 +23223,7 @@
         <v>2734.7369999999996</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -23219,7 +23240,7 @@
         <v>2734.7049999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -23238,7 +23259,7 @@
         <v>2734.6659999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>70</v>
       </c>
@@ -23256,7 +23277,7 @@
         <v>2734.7939999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f>A10+10</f>
         <v>80</v>
@@ -23273,7 +23294,7 @@
         <v>2734.5979999999995</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" ref="A13:A29" si="2">A12+10</f>
         <v>90</v>
@@ -23290,7 +23311,7 @@
         <v>2734.5749999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -23307,7 +23328,7 @@
         <v>2734.5349999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="2"/>
         <v>110</v>
@@ -23324,7 +23345,7 @@
         <v>2734.5099999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="2"/>
         <v>120</v>
@@ -23750,7 +23771,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23761,7 +23782,7 @@
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -23783,8 +23804,11 @@
       <c r="G1" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -23803,8 +23827,12 @@
         <f>$F$2-C2</f>
         <v>2734.2670000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>A21- A33</f>
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+10</f>
         <v>10</v>
@@ -23821,7 +23849,7 @@
         <v>2734.261</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A21" si="1">A3+10</f>
         <v>20</v>
@@ -23838,7 +23866,7 @@
         <v>2734.2240000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -23860,7 +23888,7 @@
         <v>2734.2060000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -23880,7 +23908,7 @@
         <v>2734.2060000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -23900,7 +23928,7 @@
         <v>2734.2060000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -23920,7 +23948,7 @@
         <v>2734.2060000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -23940,7 +23968,7 @@
         <v>2734.2060000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -23960,7 +23988,7 @@
         <v>2734.2060000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -23980,7 +24008,7 @@
         <v>2734.2060000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -23999,7 +24027,7 @@
         <v>2734.3740000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -24016,7 +24044,7 @@
         <v>2734.431</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -24032,7 +24060,7 @@
         <v>2734.46</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -24051,7 +24079,7 @@
         <v>2734.3879999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -25386,7 +25414,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="I1" sqref="I1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25397,7 +25425,7 @@
     <col min="7" max="7" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -25419,8 +25447,11 @@
       <c r="G1" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -25439,8 +25470,12 @@
         <f>$F$2-C2</f>
         <v>2736.3030000000003</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>A22- A32</f>
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+10</f>
         <v>10</v>
@@ -25457,7 +25492,7 @@
         <v>2736.1690000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A35" si="1">A3+10</f>
         <v>20</v>
@@ -25474,7 +25509,7 @@
         <v>2736.1770000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -25491,7 +25526,7 @@
         <v>2736.1330000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -25508,7 +25543,7 @@
         <v>2736.1220000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -25525,7 +25560,7 @@
         <v>2736.1160000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="1"/>
         <v>60</v>
@@ -25547,7 +25582,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -25566,7 +25601,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -25586,7 +25621,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -25606,7 +25641,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -25626,7 +25661,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="1"/>
         <v>110</v>
@@ -25646,7 +25681,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="1"/>
         <v>120</v>
@@ -25666,7 +25701,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="1"/>
         <v>130</v>
@@ -25686,7 +25721,7 @@
         <v>2736.1170000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="1"/>
         <v>140</v>
@@ -26069,7 +26104,7 @@
   <dimension ref="A1:K41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26081,7 +26116,7 @@
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -26103,8 +26138,11 @@
       <c r="G1" s="10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>0</v>
       </c>
@@ -26123,8 +26161,12 @@
         <f>$F$2-C2</f>
         <v>2736.7369999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>A7- A19</f>
+        <v>-120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <f>A2+10</f>
         <v>10</v>
@@ -26141,7 +26183,7 @@
         <v>2736.7269999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <f t="shared" ref="A4:A6" si="1">A3+10</f>
         <v>20</v>
@@ -26158,7 +26200,7 @@
         <v>2736.7179999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
@@ -26175,7 +26217,7 @@
         <v>2736.6589999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -26194,7 +26236,7 @@
         <v>2736.4929999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>40</v>
       </c>
@@ -26212,7 +26254,7 @@
         <v>2736.6469999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f>A6+10</f>
         <v>50</v>
@@ -26229,7 +26271,7 @@
         <v>2736.393</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f>A8+10</f>
         <v>60</v>
@@ -26246,7 +26288,7 @@
         <v>2736.4089999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f>A9+10</f>
         <v>70</v>
@@ -26263,7 +26305,7 @@
         <v>2736.4249999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" ref="A11:A36" si="2">A10+10</f>
         <v>80</v>
@@ -26280,7 +26322,7 @@
         <v>2736.4690000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="2"/>
         <v>90</v>
@@ -26297,7 +26339,7 @@
         <v>2736.4769999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="2"/>
         <v>100</v>
@@ -26314,7 +26356,7 @@
         <v>2736.5360000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="2"/>
         <v>110</v>
@@ -26331,7 +26373,7 @@
         <v>2736.529</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="2"/>
         <v>120</v>
@@ -26348,7 +26390,7 @@
         <v>2736.5349999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="2"/>
         <v>130</v>
@@ -27958,8 +28000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15857BB-7009-42F0-BB33-F587ED47BBA2}">
   <dimension ref="A1:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28936,11 +28978,11 @@
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
       <c r="J27">
         <f t="shared" si="3"/>
         <v>2.1</v>
@@ -29007,12 +29049,12 @@
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="L30" s="24" t="s">
+      <c r="L30" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="M30" s="24"/>
-      <c r="N30" s="24"/>
-      <c r="O30" s="24"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
     </row>
     <row r="34" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
@@ -29049,8 +29091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{278C6A75-EB2C-4F06-8258-6CEC79F84880}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29375,7 +29417,7 @@
         <v>2721.9399999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="1"/>
         <v>150</v>
@@ -29395,7 +29437,7 @@
         <v>2721.9399999999996</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="1"/>
         <v>160</v>
@@ -29415,7 +29457,7 @@
         <v>2721.9399999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="1"/>
         <v>170</v>
@@ -29437,7 +29479,7 @@
         <v>2721.9399999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="1"/>
         <v>180</v>
@@ -29454,7 +29496,7 @@
         <v>2721.9809999999993</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="1"/>
         <v>190</v>
@@ -29471,7 +29513,7 @@
         <v>2721.9959999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="1"/>
         <v>200</v>
@@ -29488,7 +29530,7 @@
         <v>2721.9899999999993</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="1"/>
         <v>210</v>
@@ -29509,7 +29551,7 @@
         <v>0.19700000000011642</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="1"/>
         <v>220</v>
@@ -29526,7 +29568,7 @@
         <v>2722.0969999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="1"/>
         <v>230</v>
@@ -29543,7 +29585,7 @@
         <v>2722.0819999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="1"/>
         <v>240</v>
@@ -29560,7 +29602,7 @@
         <v>2722.0889999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="1"/>
         <v>250</v>
@@ -29577,7 +29619,7 @@
         <v>2722.1809999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f>A27+10</f>
         <v>260</v>
@@ -29594,7 +29636,7 @@
         <v>2722.1719999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="1"/>
         <v>270</v>
@@ -29611,7 +29653,7 @@
         <v>2722.1869999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="1"/>
         <v>280</v>
@@ -29628,7 +29670,7 @@
         <v>2722.1859999999992</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="1"/>
         <v>290</v>
@@ -29645,7 +29687,7 @@
         <v>2722.1749999999993</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="1"/>
         <v>300</v>
@@ -29661,6 +29703,9 @@
         <f t="shared" si="0"/>
         <v>2722.1769999999997</v>
       </c>
+      <c r="J32" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
@@ -29677,6 +29722,10 @@
       <c r="G33" s="6">
         <f t="shared" si="0"/>
         <v>2722.1909999999993</v>
+      </c>
+      <c r="J33">
+        <f>A37-A19</f>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
@@ -29871,8 +29920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF970D2A-25F7-43D8-9437-28DE93019D3F}">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30182,7 +30231,7 @@
         <v>2722.4209999999994</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="2"/>
         <v>140</v>
@@ -30199,7 +30248,7 @@
         <v>2722.4299999999994</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="2"/>
         <v>150</v>
@@ -30216,7 +30265,7 @@
         <v>2722.4159999999993</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="2"/>
         <v>160</v>
@@ -30232,8 +30281,11 @@
         <f t="shared" si="0"/>
         <v>2722.4199999999996</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="2"/>
         <v>170</v>
@@ -30249,8 +30301,12 @@
         <f t="shared" si="0"/>
         <v>2722.4179999999997</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f>A33-A10</f>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="2"/>
         <v>180</v>
@@ -30267,7 +30323,7 @@
         <v>2722.4109999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="2"/>
         <v>190</v>
@@ -30284,7 +30340,7 @@
         <v>2722.4189999999994</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="2"/>
         <v>200</v>
@@ -30301,7 +30357,7 @@
         <v>2722.4269999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="2"/>
         <v>210</v>
@@ -30318,7 +30374,7 @@
         <v>2722.4169999999995</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="2"/>
         <v>220</v>
@@ -30335,7 +30391,7 @@
         <v>2722.3849999999993</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="2"/>
         <v>230</v>
@@ -30352,7 +30408,7 @@
         <v>2722.3639999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="2"/>
         <v>240</v>
@@ -30369,7 +30425,7 @@
         <v>2722.3919999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="2"/>
         <v>250</v>
@@ -30386,7 +30442,7 @@
         <v>2722.3609999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="2"/>
         <v>260</v>
@@ -30403,7 +30459,7 @@
         <v>2722.3389999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="2"/>
         <v>270</v>
@@ -30420,7 +30476,7 @@
         <v>2722.3169999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="2"/>
         <v>280</v>
@@ -30437,7 +30493,7 @@
         <v>2722.3099999999995</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="2"/>
         <v>290</v>
@@ -31016,7 +31072,7 @@
         <f t="shared" si="0"/>
         <v>2722.5989999999997</v>
       </c>
-      <c r="J4" s="22">
+      <c r="J4" s="5">
         <f>K4/100</f>
         <v>0.1</v>
       </c>
@@ -31053,7 +31109,7 @@
         <f t="shared" si="0"/>
         <v>2722.5309999999999</v>
       </c>
-      <c r="J5" s="22">
+      <c r="J5" s="5">
         <f t="shared" ref="J5:J24" si="3">K5/100</f>
         <v>0.2</v>
       </c>
@@ -31088,7 +31144,7 @@
         <f t="shared" si="0"/>
         <v>2722.5299999999997</v>
       </c>
-      <c r="J6" s="22">
+      <c r="J6" s="5">
         <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
@@ -31123,7 +31179,7 @@
         <f t="shared" si="0"/>
         <v>2722.5149999999999</v>
       </c>
-      <c r="J7" s="22">
+      <c r="J7" s="5">
         <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
@@ -31158,7 +31214,7 @@
         <f t="shared" si="0"/>
         <v>2722.4839999999999</v>
       </c>
-      <c r="J8" s="22">
+      <c r="J8" s="5">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -31193,7 +31249,7 @@
         <f t="shared" si="0"/>
         <v>2722.5140000000001</v>
       </c>
-      <c r="J9" s="22">
+      <c r="J9" s="5">
         <f t="shared" si="3"/>
         <v>0.6</v>
       </c>
@@ -31234,7 +31290,7 @@
         <f t="shared" si="0"/>
         <v>2722.509</v>
       </c>
-      <c r="J10" s="22">
+      <c r="J10" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
@@ -31278,7 +31334,7 @@
         <f t="shared" si="0"/>
         <v>2722.5009999999997</v>
       </c>
-      <c r="J11" s="22">
+      <c r="J11" s="5">
         <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
@@ -31315,7 +31371,7 @@
         <f t="shared" si="0"/>
         <v>2722.0859999999998</v>
       </c>
-      <c r="J12" s="22">
+      <c r="J12" s="5">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
@@ -31350,7 +31406,7 @@
       <c r="I13" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="J13" s="22">
+      <c r="J13" s="5">
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
@@ -31391,7 +31447,7 @@
         <f>G15-G14</f>
         <v>0.13900000000012369</v>
       </c>
-      <c r="J14" s="22">
+      <c r="J14" s="5">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -31427,7 +31483,7 @@
         <f t="shared" ref="G15:G31" si="4">$F$2-C15</f>
         <v>2722.652</v>
       </c>
-      <c r="J15" s="22">
+      <c r="J15" s="5">
         <f t="shared" si="3"/>
         <v>1.1000000000000001</v>
       </c>
@@ -31465,7 +31521,7 @@
       <c r="I16" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="J16" s="22">
+      <c r="J16" s="5">
         <f t="shared" si="3"/>
         <v>1.2</v>
       </c>
@@ -31504,7 +31560,7 @@
         <f>M10-M11</f>
         <v>0.19399999999999995</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="5">
         <f t="shared" si="3"/>
         <v>1.3</v>
       </c>
@@ -31541,7 +31597,7 @@
         <f t="shared" si="4"/>
         <v>2722.502</v>
       </c>
-      <c r="J18" s="22">
+      <c r="J18" s="5">
         <f t="shared" si="3"/>
         <v>1.4</v>
       </c>
@@ -31580,7 +31636,7 @@
         <f>0.4-I17</f>
         <v>0.20600000000000007</v>
       </c>
-      <c r="J19" s="22">
+      <c r="J19" s="5">
         <f t="shared" si="3"/>
         <v>1.5</v>
       </c>
@@ -31617,7 +31673,7 @@
         <f t="shared" si="4"/>
         <v>2722.5319999999997</v>
       </c>
-      <c r="J20" s="22">
+      <c r="J20" s="5">
         <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
@@ -31652,7 +31708,7 @@
         <f t="shared" si="4"/>
         <v>2722.558</v>
       </c>
-      <c r="J21" s="22">
+      <c r="J21" s="5">
         <f t="shared" si="3"/>
         <v>1.7</v>
       </c>
@@ -31687,7 +31743,7 @@
         <f t="shared" si="4"/>
         <v>2722.5569999999998</v>
       </c>
-      <c r="J22" s="22">
+      <c r="J22" s="5">
         <f t="shared" si="3"/>
         <v>1.8</v>
       </c>
@@ -31722,7 +31778,7 @@
         <f t="shared" si="4"/>
         <v>2722.5909999999999</v>
       </c>
-      <c r="J23" s="22">
+      <c r="J23" s="5">
         <f t="shared" si="3"/>
         <v>1.9</v>
       </c>
@@ -31757,7 +31813,7 @@
         <f t="shared" si="4"/>
         <v>2722.5720000000001</v>
       </c>
-      <c r="J24" s="22">
+      <c r="J24" s="5">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
@@ -31809,13 +31865,13 @@
         <f t="shared" si="4"/>
         <v>2722.5949999999998</v>
       </c>
-      <c r="K26" s="24" t="s">
+      <c r="K26" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="L26" s="24"/>
-      <c r="M26" s="24"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="23" t="s">
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="22" t="s">
         <v>124</v>
       </c>
     </row>
@@ -31835,7 +31891,7 @@
         <f t="shared" si="4"/>
         <v>2722.605</v>
       </c>
-      <c r="O27" s="23"/>
+      <c r="O27" s="22"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
@@ -31855,7 +31911,7 @@
         <f t="shared" si="4"/>
         <v>2722.8269999999998</v>
       </c>
-      <c r="O28" s="23"/>
+      <c r="O28" s="22"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
@@ -31873,7 +31929,7 @@
         <f t="shared" si="4"/>
         <v>2722.8319999999999</v>
       </c>
-      <c r="O29" s="23"/>
+      <c r="O29" s="22"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
@@ -31891,7 +31947,7 @@
         <f t="shared" si="4"/>
         <v>2722.8669999999997</v>
       </c>
-      <c r="O30" s="23"/>
+      <c r="O30" s="22"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
@@ -31913,11 +31969,11 @@
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="23" t="s">
         <v>128</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -31934,7 +31990,7 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31988,6 +32044,9 @@
         <f>$F$2-C2</f>
         <v>2722.9960000000001</v>
       </c>
+      <c r="I2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -32004,6 +32063,10 @@
       <c r="G3" s="6">
         <f t="shared" ref="G3:G32" si="0">$F$2-C3</f>
         <v>2722.9549999999999</v>
+      </c>
+      <c r="I3">
+        <f>A26-A16</f>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>